<commit_message>
Analysis Antera 2nd round
</commit_message>
<xml_diff>
--- a/Data/Antera_inputs_v2.xlsx
+++ b/Data/Antera_inputs_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giparoli\Documents\Projetos\AEco\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F519CA48-6812-4377-AACE-83792A41E7FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADFA74C1-55C9-4A7C-A95E-304479A7CA78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32025" yWindow="3315" windowWidth="17280" windowHeight="9075" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Antera_spray_etanol" sheetId="11" r:id="rId1"/>
@@ -1401,7 +1401,7 @@
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1455,12 +1455,6 @@
       <sz val="11"/>
       <color rgb="FFC00000"/>
       <name val="Calibri (Body)"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="12">
@@ -1804,6 +1798,9 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -1854,9 +1851,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2375,14 +2369,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="B1" s="66" t="s">
+      <c r="B1" s="67" t="s">
         <v>212</v>
       </c>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
     </row>
     <row r="2" spans="1:7">
       <c r="B2" s="28"/>
@@ -2413,7 +2407,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1">
-      <c r="A4" s="68" t="s">
+      <c r="A4" s="69" t="s">
         <v>37</v>
       </c>
       <c r="B4" s="8" t="s">
@@ -2438,7 +2432,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1">
-      <c r="A5" s="68"/>
+      <c r="A5" s="69"/>
       <c r="B5" s="8" t="s">
         <v>185</v>
       </c>
@@ -2461,7 +2455,7 @@
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="68"/>
+      <c r="A6" s="69"/>
       <c r="B6" s="8" t="s">
         <v>5</v>
       </c>
@@ -2484,7 +2478,7 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="68"/>
+      <c r="A7" s="69"/>
       <c r="B7" s="8" t="s">
         <v>125</v>
       </c>
@@ -2507,7 +2501,7 @@
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="68"/>
+      <c r="A8" s="69"/>
       <c r="B8" s="8" t="s">
         <v>126</v>
       </c>
@@ -2531,7 +2525,7 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="68"/>
+      <c r="A9" s="69"/>
       <c r="B9" s="8" t="s">
         <v>127</v>
       </c>
@@ -2554,7 +2548,7 @@
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="68"/>
+      <c r="A10" s="69"/>
       <c r="B10" s="8" t="s">
         <v>54</v>
       </c>
@@ -2578,7 +2572,7 @@
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="68"/>
+      <c r="A11" s="69"/>
       <c r="B11" s="8" t="s">
         <v>134</v>
       </c>
@@ -2602,7 +2596,7 @@
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="68"/>
+      <c r="A12" s="69"/>
       <c r="B12" s="8" t="s">
         <v>121</v>
       </c>
@@ -2626,7 +2620,7 @@
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="68"/>
+      <c r="A13" s="69"/>
       <c r="B13" s="8" t="s">
         <v>128</v>
       </c>
@@ -2647,7 +2641,7 @@
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="68"/>
+      <c r="A14" s="69"/>
       <c r="B14" s="8" t="s">
         <v>129</v>
       </c>
@@ -2668,7 +2662,7 @@
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="68"/>
+      <c r="A15" s="69"/>
       <c r="B15" s="8" t="s">
         <v>130</v>
       </c>
@@ -2689,7 +2683,7 @@
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="68"/>
+      <c r="A16" s="69"/>
       <c r="B16" s="8" t="s">
         <v>131</v>
       </c>
@@ -2710,7 +2704,7 @@
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="68"/>
+      <c r="A17" s="69"/>
       <c r="B17" s="8" t="s">
         <v>132</v>
       </c>
@@ -2731,7 +2725,7 @@
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="69"/>
+      <c r="A18" s="70"/>
       <c r="B18" s="8" t="s">
         <v>133</v>
       </c>
@@ -2752,7 +2746,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" s="30" customFormat="1" ht="14.7" customHeight="1">
-      <c r="A19" s="70" t="s">
+      <c r="A19" s="71" t="s">
         <v>56</v>
       </c>
       <c r="B19" s="43" t="s">
@@ -2778,7 +2772,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" s="30" customFormat="1">
-      <c r="A20" s="71"/>
+      <c r="A20" s="72"/>
       <c r="B20" s="43" t="s">
         <v>62</v>
       </c>
@@ -2802,7 +2796,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" s="30" customFormat="1">
-      <c r="A21" s="71"/>
+      <c r="A21" s="72"/>
       <c r="B21" s="43" t="s">
         <v>63</v>
       </c>
@@ -2826,7 +2820,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="14.55" customHeight="1">
-      <c r="A22" s="72" t="s">
+      <c r="A22" s="73" t="s">
         <v>58</v>
       </c>
       <c r="B22" s="32" t="s">
@@ -2852,7 +2846,7 @@
       </c>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="73"/>
+      <c r="A23" s="74"/>
       <c r="B23" s="22" t="s">
         <v>64</v>
       </c>
@@ -2876,7 +2870,7 @@
       </c>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="73"/>
+      <c r="A24" s="74"/>
       <c r="B24" s="22" t="s">
         <v>174</v>
       </c>
@@ -2900,7 +2894,7 @@
       </c>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="73"/>
+      <c r="A25" s="74"/>
       <c r="B25" s="22" t="s">
         <v>122</v>
       </c>
@@ -2924,7 +2918,7 @@
       </c>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="73"/>
+      <c r="A26" s="74"/>
       <c r="B26" s="32" t="s">
         <v>175</v>
       </c>
@@ -2947,7 +2941,7 @@
       </c>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="73"/>
+      <c r="A27" s="74"/>
       <c r="B27" s="32" t="s">
         <v>176</v>
       </c>
@@ -2970,7 +2964,7 @@
       </c>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="73"/>
+      <c r="A28" s="74"/>
       <c r="B28" s="22" t="s">
         <v>70</v>
       </c>
@@ -2993,7 +2987,7 @@
       </c>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="73"/>
+      <c r="A29" s="74"/>
       <c r="B29" s="22" t="s">
         <v>71</v>
       </c>
@@ -3016,7 +3010,7 @@
       </c>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="73"/>
+      <c r="A30" s="74"/>
       <c r="B30" s="22" t="s">
         <v>74</v>
       </c>
@@ -3039,7 +3033,7 @@
       </c>
     </row>
     <row r="31" spans="1:7" ht="14.55" customHeight="1">
-      <c r="A31" s="74" t="s">
+      <c r="A31" s="75" t="s">
         <v>34</v>
       </c>
       <c r="B31" s="9" t="s">
@@ -3063,7 +3057,7 @@
       </c>
     </row>
     <row r="32" spans="1:7" ht="14.55" customHeight="1">
-      <c r="A32" s="75"/>
+      <c r="A32" s="76"/>
       <c r="B32" s="9" t="s">
         <v>12</v>
       </c>
@@ -3085,7 +3079,7 @@
       </c>
     </row>
     <row r="33" spans="1:13">
-      <c r="A33" s="75"/>
+      <c r="A33" s="76"/>
       <c r="B33" s="9" t="s">
         <v>142</v>
       </c>
@@ -3107,7 +3101,7 @@
       </c>
     </row>
     <row r="34" spans="1:13">
-      <c r="A34" s="75"/>
+      <c r="A34" s="76"/>
       <c r="B34" s="9" t="s">
         <v>19</v>
       </c>
@@ -3128,7 +3122,7 @@
       </c>
     </row>
     <row r="35" spans="1:13">
-      <c r="A35" s="75"/>
+      <c r="A35" s="76"/>
       <c r="B35" s="9" t="s">
         <v>13</v>
       </c>
@@ -3149,7 +3143,7 @@
       </c>
     </row>
     <row r="36" spans="1:13">
-      <c r="A36" s="75"/>
+      <c r="A36" s="76"/>
       <c r="B36" s="9" t="s">
         <v>14</v>
       </c>
@@ -3170,7 +3164,7 @@
       </c>
     </row>
     <row r="37" spans="1:13">
-      <c r="A37" s="75"/>
+      <c r="A37" s="76"/>
       <c r="B37" s="9" t="s">
         <v>15</v>
       </c>
@@ -3191,7 +3185,7 @@
       </c>
     </row>
     <row r="38" spans="1:13">
-      <c r="A38" s="75"/>
+      <c r="A38" s="76"/>
       <c r="B38" s="9" t="s">
         <v>16</v>
       </c>
@@ -3212,7 +3206,7 @@
       </c>
     </row>
     <row r="39" spans="1:13">
-      <c r="A39" s="75"/>
+      <c r="A39" s="76"/>
       <c r="B39" s="9" t="s">
         <v>146</v>
       </c>
@@ -3233,7 +3227,7 @@
       </c>
     </row>
     <row r="40" spans="1:13">
-      <c r="A40" s="75"/>
+      <c r="A40" s="76"/>
       <c r="B40" s="9" t="s">
         <v>20</v>
       </c>
@@ -3254,7 +3248,7 @@
       </c>
     </row>
     <row r="41" spans="1:13">
-      <c r="A41" s="75"/>
+      <c r="A41" s="76"/>
       <c r="B41" s="9" t="s">
         <v>17</v>
       </c>
@@ -3275,7 +3269,7 @@
       </c>
     </row>
     <row r="42" spans="1:13">
-      <c r="A42" s="75"/>
+      <c r="A42" s="76"/>
       <c r="B42" s="9" t="s">
         <v>18</v>
       </c>
@@ -3296,7 +3290,7 @@
       </c>
     </row>
     <row r="43" spans="1:13" ht="14.55" customHeight="1">
-      <c r="A43" s="76" t="s">
+      <c r="A43" s="77" t="s">
         <v>35</v>
       </c>
       <c r="B43" s="35" t="s">
@@ -3321,7 +3315,7 @@
       </c>
     </row>
     <row r="44" spans="1:13" ht="14.55" customHeight="1">
-      <c r="A44" s="77"/>
+      <c r="A44" s="78"/>
       <c r="B44" s="35" t="s">
         <v>119</v>
       </c>
@@ -3349,7 +3343,7 @@
       <c r="M44" s="51"/>
     </row>
     <row r="45" spans="1:13" ht="14.55" customHeight="1">
-      <c r="A45" s="77"/>
+      <c r="A45" s="78"/>
       <c r="B45" s="35" t="s">
         <v>120</v>
       </c>
@@ -3377,7 +3371,7 @@
       <c r="M45" s="51"/>
     </row>
     <row r="46" spans="1:13" ht="14.55" customHeight="1">
-      <c r="A46" s="77"/>
+      <c r="A46" s="78"/>
       <c r="B46" s="47" t="s">
         <v>194</v>
       </c>
@@ -3407,7 +3401,7 @@
       <c r="M46" s="51"/>
     </row>
     <row r="47" spans="1:13">
-      <c r="A47" s="77"/>
+      <c r="A47" s="78"/>
       <c r="B47" s="35" t="s">
         <v>21</v>
       </c>
@@ -3436,7 +3430,7 @@
       <c r="M47" s="51"/>
     </row>
     <row r="48" spans="1:13">
-      <c r="A48" s="77"/>
+      <c r="A48" s="78"/>
       <c r="B48" s="35" t="s">
         <v>22</v>
       </c>
@@ -3465,7 +3459,7 @@
       <c r="M48" s="51"/>
     </row>
     <row r="49" spans="1:13">
-      <c r="A49" s="77"/>
+      <c r="A49" s="78"/>
       <c r="B49" s="35" t="s">
         <v>23</v>
       </c>
@@ -3494,7 +3488,7 @@
       <c r="M49" s="51"/>
     </row>
     <row r="50" spans="1:13">
-      <c r="A50" s="78"/>
+      <c r="A50" s="79"/>
       <c r="B50" s="35" t="s">
         <v>138</v>
       </c>
@@ -3666,7 +3660,7 @@
       </c>
     </row>
     <row r="57" spans="1:13" ht="14.55" customHeight="1">
-      <c r="A57" s="79" t="s">
+      <c r="A57" s="62" t="s">
         <v>33</v>
       </c>
       <c r="B57" s="17" t="s">
@@ -3693,7 +3687,7 @@
       <c r="K57" s="13"/>
     </row>
     <row r="58" spans="1:13">
-      <c r="A58" s="62"/>
+      <c r="A58" s="63"/>
       <c r="B58" s="17" t="s">
         <v>151</v>
       </c>
@@ -3718,7 +3712,7 @@
       <c r="K58" s="13"/>
     </row>
     <row r="59" spans="1:13">
-      <c r="A59" s="62"/>
+      <c r="A59" s="63"/>
       <c r="B59" s="17" t="s">
         <v>197</v>
       </c>
@@ -3743,7 +3737,7 @@
       <c r="K59" s="13"/>
     </row>
     <row r="60" spans="1:13">
-      <c r="A60" s="62"/>
+      <c r="A60" s="63"/>
       <c r="B60" s="17" t="s">
         <v>198</v>
       </c>
@@ -3764,7 +3758,7 @@
       <c r="K60" s="13"/>
     </row>
     <row r="61" spans="1:13">
-      <c r="A61" s="62"/>
+      <c r="A61" s="63"/>
       <c r="B61" s="17" t="s">
         <v>199</v>
       </c>
@@ -3785,7 +3779,7 @@
       <c r="K61" s="13"/>
     </row>
     <row r="62" spans="1:13">
-      <c r="A62" s="62"/>
+      <c r="A62" s="63"/>
       <c r="B62" s="17" t="s">
         <v>210</v>
       </c>
@@ -3810,7 +3804,7 @@
       <c r="K62" s="13"/>
     </row>
     <row r="63" spans="1:13">
-      <c r="A63" s="62"/>
+      <c r="A63" s="63"/>
       <c r="B63" s="17" t="s">
         <v>155</v>
       </c>
@@ -3835,7 +3829,7 @@
       <c r="K63" s="13"/>
     </row>
     <row r="64" spans="1:13">
-      <c r="A64" s="62"/>
+      <c r="A64" s="63"/>
       <c r="B64" s="20" t="s">
         <v>200</v>
       </c>
@@ -3859,7 +3853,7 @@
       </c>
     </row>
     <row r="65" spans="1:11">
-      <c r="A65" s="62"/>
+      <c r="A65" s="63"/>
       <c r="B65" s="20" t="s">
         <v>201</v>
       </c>
@@ -3879,7 +3873,7 @@
       <c r="G65" s="19"/>
     </row>
     <row r="66" spans="1:11">
-      <c r="A66" s="62"/>
+      <c r="A66" s="63"/>
       <c r="B66" s="20" t="s">
         <v>202</v>
       </c>
@@ -3899,7 +3893,7 @@
       <c r="G66" s="19"/>
     </row>
     <row r="67" spans="1:11">
-      <c r="A67" s="62"/>
+      <c r="A67" s="63"/>
       <c r="B67" s="20" t="s">
         <v>117</v>
       </c>
@@ -3923,7 +3917,7 @@
       <c r="K67" s="13"/>
     </row>
     <row r="68" spans="1:11">
-      <c r="A68" s="62"/>
+      <c r="A68" s="63"/>
       <c r="B68" s="20" t="s">
         <v>203</v>
       </c>
@@ -3946,7 +3940,7 @@
       <c r="K68" s="13"/>
     </row>
     <row r="69" spans="1:11" ht="14.55" customHeight="1">
-      <c r="A69" s="62"/>
+      <c r="A69" s="63"/>
       <c r="B69" s="20" t="s">
         <v>159</v>
       </c>
@@ -3968,7 +3962,7 @@
       <c r="K69" s="13"/>
     </row>
     <row r="70" spans="1:11" ht="14.55" customHeight="1">
-      <c r="A70" s="62"/>
+      <c r="A70" s="63"/>
       <c r="B70" s="20" t="s">
         <v>204</v>
       </c>
@@ -3988,7 +3982,7 @@
       <c r="K70" s="13"/>
     </row>
     <row r="71" spans="1:11" ht="14.55" customHeight="1">
-      <c r="A71" s="62"/>
+      <c r="A71" s="63"/>
       <c r="B71" s="20" t="s">
         <v>206</v>
       </c>
@@ -4012,7 +4006,7 @@
       <c r="K71" s="13"/>
     </row>
     <row r="72" spans="1:11" ht="14.55" customHeight="1">
-      <c r="A72" s="62"/>
+      <c r="A72" s="63"/>
       <c r="B72" s="20" t="s">
         <v>207</v>
       </c>
@@ -4035,7 +4029,7 @@
       <c r="K72" s="13"/>
     </row>
     <row r="73" spans="1:11" ht="14.55" customHeight="1">
-      <c r="A73" s="62"/>
+      <c r="A73" s="63"/>
       <c r="B73" s="17" t="s">
         <v>161</v>
       </c>
@@ -4059,7 +4053,7 @@
       <c r="K73" s="13"/>
     </row>
     <row r="74" spans="1:11">
-      <c r="A74" s="62"/>
+      <c r="A74" s="63"/>
       <c r="B74" s="17" t="s">
         <v>162</v>
       </c>
@@ -4083,7 +4077,7 @@
       <c r="K74" s="13"/>
     </row>
     <row r="75" spans="1:11">
-      <c r="A75" s="62"/>
+      <c r="A75" s="63"/>
       <c r="B75" s="17" t="s">
         <v>164</v>
       </c>
@@ -4107,7 +4101,7 @@
       <c r="K75" s="13"/>
     </row>
     <row r="76" spans="1:11">
-      <c r="A76" s="63"/>
+      <c r="A76" s="64"/>
       <c r="B76" s="17" t="s">
         <v>76</v>
       </c>
@@ -4131,7 +4125,7 @@
       <c r="K76" s="13"/>
     </row>
     <row r="77" spans="1:11" ht="14.55" customHeight="1">
-      <c r="A77" s="64" t="s">
+      <c r="A77" s="65" t="s">
         <v>38</v>
       </c>
       <c r="B77" s="40" t="s">
@@ -4154,7 +4148,7 @@
       </c>
     </row>
     <row r="78" spans="1:11">
-      <c r="A78" s="65"/>
+      <c r="A78" s="66"/>
       <c r="B78" s="40" t="s">
         <v>48</v>
       </c>
@@ -4175,7 +4169,7 @@
       </c>
     </row>
     <row r="79" spans="1:11">
-      <c r="A79" s="65"/>
+      <c r="A79" s="66"/>
       <c r="B79" s="40" t="s">
         <v>40</v>
       </c>
@@ -4196,7 +4190,7 @@
       </c>
     </row>
     <row r="80" spans="1:11">
-      <c r="A80" s="65"/>
+      <c r="A80" s="66"/>
       <c r="B80" s="40" t="s">
         <v>41</v>
       </c>
@@ -4217,7 +4211,7 @@
       </c>
     </row>
     <row r="81" spans="1:11">
-      <c r="A81" s="65"/>
+      <c r="A81" s="66"/>
       <c r="B81" s="40" t="s">
         <v>42</v>
       </c>
@@ -4238,7 +4232,7 @@
       </c>
     </row>
     <row r="82" spans="1:11">
-      <c r="A82" s="65"/>
+      <c r="A82" s="66"/>
       <c r="B82" s="40" t="s">
         <v>188</v>
       </c>
@@ -4260,7 +4254,7 @@
       <c r="K82" s="13"/>
     </row>
     <row r="83" spans="1:11">
-      <c r="A83" s="65"/>
+      <c r="A83" s="66"/>
       <c r="B83" s="40" t="s">
         <v>43</v>
       </c>
@@ -4282,7 +4276,7 @@
       <c r="K83" s="13"/>
     </row>
     <row r="84" spans="1:11">
-      <c r="A84" s="65"/>
+      <c r="A84" s="66"/>
       <c r="B84" s="40" t="s">
         <v>49</v>
       </c>
@@ -4304,7 +4298,7 @@
       <c r="K84" s="13"/>
     </row>
     <row r="85" spans="1:11">
-      <c r="A85" s="65"/>
+      <c r="A85" s="66"/>
       <c r="B85" s="40" t="s">
         <v>44</v>
       </c>
@@ -4326,7 +4320,7 @@
       <c r="K85" s="13"/>
     </row>
     <row r="86" spans="1:11">
-      <c r="A86" s="65"/>
+      <c r="A86" s="66"/>
       <c r="B86" s="40" t="s">
         <v>45</v>
       </c>
@@ -4348,7 +4342,7 @@
       <c r="K86" s="13"/>
     </row>
     <row r="87" spans="1:11">
-      <c r="A87" s="65"/>
+      <c r="A87" s="66"/>
       <c r="B87" s="40" t="s">
         <v>46</v>
       </c>
@@ -4369,7 +4363,7 @@
       </c>
     </row>
     <row r="88" spans="1:11">
-      <c r="A88" s="65"/>
+      <c r="A88" s="66"/>
       <c r="B88" s="40" t="s">
         <v>189</v>
       </c>
@@ -4390,7 +4384,7 @@
       </c>
     </row>
     <row r="89" spans="1:11">
-      <c r="A89" s="65"/>
+      <c r="A89" s="66"/>
       <c r="B89" s="40" t="s">
         <v>47</v>
       </c>
@@ -4411,7 +4405,7 @@
       </c>
     </row>
     <row r="90" spans="1:11">
-      <c r="A90" s="65"/>
+      <c r="A90" s="66"/>
       <c r="B90" s="40" t="s">
         <v>50</v>
       </c>
@@ -4432,7 +4426,7 @@
       </c>
     </row>
     <row r="91" spans="1:11">
-      <c r="A91" s="65"/>
+      <c r="A91" s="66"/>
       <c r="B91" s="40" t="s">
         <v>51</v>
       </c>
@@ -4453,7 +4447,7 @@
       </c>
     </row>
     <row r="92" spans="1:11">
-      <c r="A92" s="65"/>
+      <c r="A92" s="66"/>
       <c r="B92" s="40" t="s">
         <v>52</v>
       </c>
@@ -4474,7 +4468,7 @@
       </c>
     </row>
     <row r="93" spans="1:11">
-      <c r="A93" s="65"/>
+      <c r="A93" s="66"/>
       <c r="B93" s="40" t="s">
         <v>53</v>
       </c>
@@ -4496,7 +4490,7 @@
       <c r="K93" s="13"/>
     </row>
     <row r="94" spans="1:11">
-      <c r="A94" s="65"/>
+      <c r="A94" s="66"/>
       <c r="B94" s="40" t="s">
         <v>190</v>
       </c>
@@ -4585,7 +4579,7 @@
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C43" sqref="C43"/>
+      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -4597,19 +4591,20 @@
     <col min="5" max="5" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="75.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="B1" s="66" t="s">
+    <row r="1" spans="1:9">
+      <c r="B1" s="67" t="s">
         <v>212</v>
       </c>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+    </row>
+    <row r="2" spans="1:9">
       <c r="B2" s="28"/>
       <c r="C2" s="29"/>
       <c r="D2" s="29"/>
@@ -4617,7 +4612,7 @@
       <c r="F2" s="29"/>
       <c r="G2" s="29"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:9">
       <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
@@ -4637,8 +4632,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15" customHeight="1">
-      <c r="A4" s="68" t="s">
+    <row r="4" spans="1:9" ht="15" customHeight="1">
+      <c r="A4" s="69" t="s">
         <v>37</v>
       </c>
       <c r="B4" s="8" t="s">
@@ -4662,8 +4657,8 @@
         <v>186</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15" customHeight="1">
-      <c r="A5" s="68"/>
+    <row r="5" spans="1:9" ht="15" customHeight="1">
+      <c r="A5" s="69"/>
       <c r="B5" s="8" t="s">
         <v>185</v>
       </c>
@@ -4685,8 +4680,8 @@
         <v>187</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="68"/>
+    <row r="6" spans="1:9">
+      <c r="A6" s="69"/>
       <c r="B6" s="8" t="s">
         <v>5</v>
       </c>
@@ -4708,8 +4703,8 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="68"/>
+    <row r="7" spans="1:9">
+      <c r="A7" s="69"/>
       <c r="B7" s="8" t="s">
         <v>125</v>
       </c>
@@ -4731,8 +4726,8 @@
         <v>183</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="68"/>
+    <row r="8" spans="1:9">
+      <c r="A8" s="69"/>
       <c r="B8" s="8" t="s">
         <v>126</v>
       </c>
@@ -4754,9 +4749,13 @@
       <c r="G8" s="3" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="68"/>
+      <c r="I8">
+        <f>C7*C8*C9*C10*(C11+C12)</f>
+        <v>5857481725.1626673</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="69"/>
       <c r="B9" s="8" t="s">
         <v>127</v>
       </c>
@@ -4777,9 +4776,13 @@
       <c r="G9" s="3" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="68"/>
+      <c r="I9">
+        <f>C7*C8*C9*C10</f>
+        <v>713978.75733333337</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="69"/>
       <c r="B10" s="8" t="s">
         <v>54</v>
       </c>
@@ -4802,8 +4805,8 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="68"/>
+    <row r="11" spans="1:9">
+      <c r="A11" s="69"/>
       <c r="B11" s="8" t="s">
         <v>134</v>
       </c>
@@ -4826,8 +4829,8 @@
         <v>172</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="68"/>
+    <row r="12" spans="1:9">
+      <c r="A12" s="69"/>
       <c r="B12" s="8" t="s">
         <v>121</v>
       </c>
@@ -4850,8 +4853,8 @@
         <v>173</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="68"/>
+    <row r="13" spans="1:9">
+      <c r="A13" s="69"/>
       <c r="B13" s="8" t="s">
         <v>128</v>
       </c>
@@ -4871,8 +4874,8 @@
         <v>166</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="68"/>
+    <row r="14" spans="1:9">
+      <c r="A14" s="69"/>
       <c r="B14" s="8" t="s">
         <v>129</v>
       </c>
@@ -4892,8 +4895,8 @@
         <v>167</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="68"/>
+    <row r="15" spans="1:9">
+      <c r="A15" s="69"/>
       <c r="B15" s="8" t="s">
         <v>130</v>
       </c>
@@ -4913,8 +4916,8 @@
         <v>168</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="68"/>
+    <row r="16" spans="1:9">
+      <c r="A16" s="69"/>
       <c r="B16" s="8" t="s">
         <v>131</v>
       </c>
@@ -4935,7 +4938,7 @@
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="68"/>
+      <c r="A17" s="69"/>
       <c r="B17" s="8" t="s">
         <v>132</v>
       </c>
@@ -4956,7 +4959,7 @@
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="69"/>
+      <c r="A18" s="70"/>
       <c r="B18" s="8" t="s">
         <v>133</v>
       </c>
@@ -4977,7 +4980,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" s="30" customFormat="1" ht="14.7" customHeight="1">
-      <c r="A19" s="70" t="s">
+      <c r="A19" s="71" t="s">
         <v>56</v>
       </c>
       <c r="B19" s="43" t="s">
@@ -5003,7 +5006,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" s="30" customFormat="1">
-      <c r="A20" s="71"/>
+      <c r="A20" s="72"/>
       <c r="B20" s="43" t="s">
         <v>62</v>
       </c>
@@ -5027,7 +5030,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" s="30" customFormat="1">
-      <c r="A21" s="71"/>
+      <c r="A21" s="72"/>
       <c r="B21" s="43" t="s">
         <v>63</v>
       </c>
@@ -5051,7 +5054,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="14.55" customHeight="1">
-      <c r="A22" s="72" t="s">
+      <c r="A22" s="73" t="s">
         <v>58</v>
       </c>
       <c r="B22" s="32" t="s">
@@ -5077,7 +5080,7 @@
       </c>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="73"/>
+      <c r="A23" s="74"/>
       <c r="B23" s="22" t="s">
         <v>64</v>
       </c>
@@ -5101,7 +5104,7 @@
       </c>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="73"/>
+      <c r="A24" s="74"/>
       <c r="B24" s="22" t="s">
         <v>174</v>
       </c>
@@ -5125,7 +5128,7 @@
       </c>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="73"/>
+      <c r="A25" s="74"/>
       <c r="B25" s="22" t="s">
         <v>122</v>
       </c>
@@ -5149,7 +5152,7 @@
       </c>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="73"/>
+      <c r="A26" s="74"/>
       <c r="B26" s="32" t="s">
         <v>175</v>
       </c>
@@ -5172,7 +5175,7 @@
       </c>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="73"/>
+      <c r="A27" s="74"/>
       <c r="B27" s="32" t="s">
         <v>176</v>
       </c>
@@ -5195,7 +5198,7 @@
       </c>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="73"/>
+      <c r="A28" s="74"/>
       <c r="B28" s="22" t="s">
         <v>70</v>
       </c>
@@ -5218,7 +5221,7 @@
       </c>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="73"/>
+      <c r="A29" s="74"/>
       <c r="B29" s="22" t="s">
         <v>71</v>
       </c>
@@ -5241,7 +5244,7 @@
       </c>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="73"/>
+      <c r="A30" s="74"/>
       <c r="B30" s="22" t="s">
         <v>74</v>
       </c>
@@ -5264,7 +5267,7 @@
       </c>
     </row>
     <row r="31" spans="1:7" ht="14.55" customHeight="1">
-      <c r="A31" s="74" t="s">
+      <c r="A31" s="75" t="s">
         <v>34</v>
       </c>
       <c r="B31" s="9" t="s">
@@ -5288,7 +5291,7 @@
       </c>
     </row>
     <row r="32" spans="1:7" ht="14.55" customHeight="1">
-      <c r="A32" s="75"/>
+      <c r="A32" s="76"/>
       <c r="B32" s="9" t="s">
         <v>12</v>
       </c>
@@ -5310,7 +5313,7 @@
       </c>
     </row>
     <row r="33" spans="1:13">
-      <c r="A33" s="75"/>
+      <c r="A33" s="76"/>
       <c r="B33" s="9" t="s">
         <v>142</v>
       </c>
@@ -5332,7 +5335,7 @@
       </c>
     </row>
     <row r="34" spans="1:13">
-      <c r="A34" s="75"/>
+      <c r="A34" s="76"/>
       <c r="B34" s="9" t="s">
         <v>19</v>
       </c>
@@ -5353,7 +5356,7 @@
       </c>
     </row>
     <row r="35" spans="1:13">
-      <c r="A35" s="75"/>
+      <c r="A35" s="76"/>
       <c r="B35" s="9" t="s">
         <v>13</v>
       </c>
@@ -5374,7 +5377,7 @@
       </c>
     </row>
     <row r="36" spans="1:13">
-      <c r="A36" s="75"/>
+      <c r="A36" s="76"/>
       <c r="B36" s="9" t="s">
         <v>14</v>
       </c>
@@ -5395,7 +5398,7 @@
       </c>
     </row>
     <row r="37" spans="1:13">
-      <c r="A37" s="75"/>
+      <c r="A37" s="76"/>
       <c r="B37" s="9" t="s">
         <v>15</v>
       </c>
@@ -5416,7 +5419,7 @@
       </c>
     </row>
     <row r="38" spans="1:13">
-      <c r="A38" s="75"/>
+      <c r="A38" s="76"/>
       <c r="B38" s="9" t="s">
         <v>16</v>
       </c>
@@ -5437,7 +5440,7 @@
       </c>
     </row>
     <row r="39" spans="1:13">
-      <c r="A39" s="75"/>
+      <c r="A39" s="76"/>
       <c r="B39" s="9" t="s">
         <v>146</v>
       </c>
@@ -5458,7 +5461,7 @@
       </c>
     </row>
     <row r="40" spans="1:13">
-      <c r="A40" s="75"/>
+      <c r="A40" s="76"/>
       <c r="B40" s="9" t="s">
         <v>20</v>
       </c>
@@ -5479,7 +5482,7 @@
       </c>
     </row>
     <row r="41" spans="1:13">
-      <c r="A41" s="75"/>
+      <c r="A41" s="76"/>
       <c r="B41" s="9" t="s">
         <v>17</v>
       </c>
@@ -5500,7 +5503,7 @@
       </c>
     </row>
     <row r="42" spans="1:13">
-      <c r="A42" s="75"/>
+      <c r="A42" s="76"/>
       <c r="B42" s="9" t="s">
         <v>18</v>
       </c>
@@ -5521,7 +5524,7 @@
       </c>
     </row>
     <row r="43" spans="1:13" ht="14.55" customHeight="1">
-      <c r="A43" s="76" t="s">
+      <c r="A43" s="77" t="s">
         <v>35</v>
       </c>
       <c r="B43" s="35" t="s">
@@ -5546,7 +5549,7 @@
       </c>
     </row>
     <row r="44" spans="1:13" ht="14.55" customHeight="1">
-      <c r="A44" s="77"/>
+      <c r="A44" s="78"/>
       <c r="B44" s="35" t="s">
         <v>119</v>
       </c>
@@ -5574,7 +5577,7 @@
       <c r="M44" s="51"/>
     </row>
     <row r="45" spans="1:13" ht="14.55" customHeight="1">
-      <c r="A45" s="77"/>
+      <c r="A45" s="78"/>
       <c r="B45" s="35" t="s">
         <v>120</v>
       </c>
@@ -5602,7 +5605,7 @@
       <c r="M45" s="51"/>
     </row>
     <row r="46" spans="1:13" ht="14.55" customHeight="1">
-      <c r="A46" s="77"/>
+      <c r="A46" s="78"/>
       <c r="B46" s="47" t="s">
         <v>194</v>
       </c>
@@ -5632,7 +5635,7 @@
       <c r="M46" s="51"/>
     </row>
     <row r="47" spans="1:13">
-      <c r="A47" s="77"/>
+      <c r="A47" s="78"/>
       <c r="B47" s="35" t="s">
         <v>21</v>
       </c>
@@ -5661,7 +5664,7 @@
       <c r="M47" s="51"/>
     </row>
     <row r="48" spans="1:13">
-      <c r="A48" s="77"/>
+      <c r="A48" s="78"/>
       <c r="B48" s="35" t="s">
         <v>22</v>
       </c>
@@ -5690,7 +5693,7 @@
       <c r="M48" s="51"/>
     </row>
     <row r="49" spans="1:13">
-      <c r="A49" s="77"/>
+      <c r="A49" s="78"/>
       <c r="B49" s="35" t="s">
         <v>23</v>
       </c>
@@ -5719,7 +5722,7 @@
       <c r="M49" s="51"/>
     </row>
     <row r="50" spans="1:13">
-      <c r="A50" s="78"/>
+      <c r="A50" s="79"/>
       <c r="B50" s="35" t="s">
         <v>138</v>
       </c>
@@ -5891,7 +5894,7 @@
       </c>
     </row>
     <row r="57" spans="1:13" ht="14.55" customHeight="1">
-      <c r="A57" s="79" t="s">
+      <c r="A57" s="62" t="s">
         <v>33</v>
       </c>
       <c r="B57" s="17" t="s">
@@ -5918,7 +5921,7 @@
       <c r="K57" s="13"/>
     </row>
     <row r="58" spans="1:13">
-      <c r="A58" s="62"/>
+      <c r="A58" s="63"/>
       <c r="B58" s="17" t="s">
         <v>151</v>
       </c>
@@ -5943,7 +5946,7 @@
       <c r="K58" s="13"/>
     </row>
     <row r="59" spans="1:13">
-      <c r="A59" s="62"/>
+      <c r="A59" s="63"/>
       <c r="B59" s="17" t="s">
         <v>197</v>
       </c>
@@ -5968,7 +5971,7 @@
       <c r="K59" s="13"/>
     </row>
     <row r="60" spans="1:13">
-      <c r="A60" s="62"/>
+      <c r="A60" s="63"/>
       <c r="B60" s="17" t="s">
         <v>198</v>
       </c>
@@ -5989,7 +5992,7 @@
       <c r="K60" s="13"/>
     </row>
     <row r="61" spans="1:13">
-      <c r="A61" s="62"/>
+      <c r="A61" s="63"/>
       <c r="B61" s="17" t="s">
         <v>199</v>
       </c>
@@ -6010,7 +6013,7 @@
       <c r="K61" s="13"/>
     </row>
     <row r="62" spans="1:13">
-      <c r="A62" s="62"/>
+      <c r="A62" s="63"/>
       <c r="B62" s="17" t="s">
         <v>214</v>
       </c>
@@ -6035,7 +6038,7 @@
       <c r="K62" s="13"/>
     </row>
     <row r="63" spans="1:13">
-      <c r="A63" s="62"/>
+      <c r="A63" s="63"/>
       <c r="B63" s="17" t="s">
         <v>155</v>
       </c>
@@ -6060,7 +6063,7 @@
       <c r="K63" s="13"/>
     </row>
     <row r="64" spans="1:13">
-      <c r="A64" s="62"/>
+      <c r="A64" s="63"/>
       <c r="B64" s="20" t="s">
         <v>200</v>
       </c>
@@ -6084,7 +6087,7 @@
       </c>
     </row>
     <row r="65" spans="1:11">
-      <c r="A65" s="62"/>
+      <c r="A65" s="63"/>
       <c r="B65" s="20" t="s">
         <v>201</v>
       </c>
@@ -6104,7 +6107,7 @@
       <c r="G65" s="19"/>
     </row>
     <row r="66" spans="1:11">
-      <c r="A66" s="62"/>
+      <c r="A66" s="63"/>
       <c r="B66" s="20" t="s">
         <v>202</v>
       </c>
@@ -6124,7 +6127,7 @@
       <c r="G66" s="19"/>
     </row>
     <row r="67" spans="1:11">
-      <c r="A67" s="62"/>
+      <c r="A67" s="63"/>
       <c r="B67" s="20" t="s">
         <v>117</v>
       </c>
@@ -6148,7 +6151,7 @@
       <c r="K67" s="13"/>
     </row>
     <row r="68" spans="1:11" ht="14.55" customHeight="1">
-      <c r="A68" s="62"/>
+      <c r="A68" s="63"/>
       <c r="B68" s="20" t="s">
         <v>159</v>
       </c>
@@ -6169,7 +6172,7 @@
       <c r="K68" s="13"/>
     </row>
     <row r="69" spans="1:11" ht="14.55" customHeight="1">
-      <c r="A69" s="62"/>
+      <c r="A69" s="63"/>
       <c r="B69" s="20" t="s">
         <v>206</v>
       </c>
@@ -6191,7 +6194,7 @@
       <c r="K69" s="13"/>
     </row>
     <row r="70" spans="1:11" ht="14.55" customHeight="1">
-      <c r="A70" s="62"/>
+      <c r="A70" s="63"/>
       <c r="B70" s="17" t="s">
         <v>161</v>
       </c>
@@ -6215,7 +6218,7 @@
       <c r="K70" s="13"/>
     </row>
     <row r="71" spans="1:11">
-      <c r="A71" s="62"/>
+      <c r="A71" s="63"/>
       <c r="B71" s="17" t="s">
         <v>162</v>
       </c>
@@ -6239,7 +6242,7 @@
       <c r="K71" s="13"/>
     </row>
     <row r="72" spans="1:11">
-      <c r="A72" s="62"/>
+      <c r="A72" s="63"/>
       <c r="B72" s="17" t="s">
         <v>164</v>
       </c>
@@ -6263,7 +6266,7 @@
       <c r="K72" s="13"/>
     </row>
     <row r="73" spans="1:11">
-      <c r="A73" s="63"/>
+      <c r="A73" s="64"/>
       <c r="B73" s="17" t="s">
         <v>76</v>
       </c>
@@ -6287,7 +6290,7 @@
       <c r="K73" s="13"/>
     </row>
     <row r="74" spans="1:11" ht="14.55" customHeight="1">
-      <c r="A74" s="64" t="s">
+      <c r="A74" s="65" t="s">
         <v>38</v>
       </c>
       <c r="B74" s="40" t="s">
@@ -6310,7 +6313,7 @@
       </c>
     </row>
     <row r="75" spans="1:11">
-      <c r="A75" s="65"/>
+      <c r="A75" s="66"/>
       <c r="B75" s="40" t="s">
         <v>48</v>
       </c>
@@ -6331,7 +6334,7 @@
       </c>
     </row>
     <row r="76" spans="1:11">
-      <c r="A76" s="65"/>
+      <c r="A76" s="66"/>
       <c r="B76" s="40" t="s">
         <v>40</v>
       </c>
@@ -6352,7 +6355,7 @@
       </c>
     </row>
     <row r="77" spans="1:11">
-      <c r="A77" s="65"/>
+      <c r="A77" s="66"/>
       <c r="B77" s="40" t="s">
         <v>41</v>
       </c>
@@ -6373,7 +6376,7 @@
       </c>
     </row>
     <row r="78" spans="1:11">
-      <c r="A78" s="65"/>
+      <c r="A78" s="66"/>
       <c r="B78" s="40" t="s">
         <v>42</v>
       </c>
@@ -6394,7 +6397,7 @@
       </c>
     </row>
     <row r="79" spans="1:11">
-      <c r="A79" s="65"/>
+      <c r="A79" s="66"/>
       <c r="B79" s="40" t="s">
         <v>188</v>
       </c>
@@ -6416,7 +6419,7 @@
       <c r="K79" s="13"/>
     </row>
     <row r="80" spans="1:11">
-      <c r="A80" s="65"/>
+      <c r="A80" s="66"/>
       <c r="B80" s="40" t="s">
         <v>43</v>
       </c>
@@ -6438,7 +6441,7 @@
       <c r="K80" s="13"/>
     </row>
     <row r="81" spans="1:11">
-      <c r="A81" s="65"/>
+      <c r="A81" s="66"/>
       <c r="B81" s="40" t="s">
         <v>49</v>
       </c>
@@ -6460,7 +6463,7 @@
       <c r="K81" s="13"/>
     </row>
     <row r="82" spans="1:11">
-      <c r="A82" s="65"/>
+      <c r="A82" s="66"/>
       <c r="B82" s="40" t="s">
         <v>44</v>
       </c>
@@ -6482,7 +6485,7 @@
       <c r="K82" s="13"/>
     </row>
     <row r="83" spans="1:11">
-      <c r="A83" s="65"/>
+      <c r="A83" s="66"/>
       <c r="B83" s="40" t="s">
         <v>45</v>
       </c>
@@ -6504,7 +6507,7 @@
       <c r="K83" s="13"/>
     </row>
     <row r="84" spans="1:11">
-      <c r="A84" s="65"/>
+      <c r="A84" s="66"/>
       <c r="B84" s="40" t="s">
         <v>46</v>
       </c>
@@ -6525,7 +6528,7 @@
       </c>
     </row>
     <row r="85" spans="1:11">
-      <c r="A85" s="65"/>
+      <c r="A85" s="66"/>
       <c r="B85" s="40" t="s">
         <v>189</v>
       </c>
@@ -6546,7 +6549,7 @@
       </c>
     </row>
     <row r="86" spans="1:11">
-      <c r="A86" s="65"/>
+      <c r="A86" s="66"/>
       <c r="B86" s="40" t="s">
         <v>47</v>
       </c>
@@ -6567,7 +6570,7 @@
       </c>
     </row>
     <row r="87" spans="1:11">
-      <c r="A87" s="65"/>
+      <c r="A87" s="66"/>
       <c r="B87" s="40" t="s">
         <v>50</v>
       </c>
@@ -6588,7 +6591,7 @@
       </c>
     </row>
     <row r="88" spans="1:11">
-      <c r="A88" s="65"/>
+      <c r="A88" s="66"/>
       <c r="B88" s="40" t="s">
         <v>51</v>
       </c>
@@ -6609,7 +6612,7 @@
       </c>
     </row>
     <row r="89" spans="1:11">
-      <c r="A89" s="65"/>
+      <c r="A89" s="66"/>
       <c r="B89" s="40" t="s">
         <v>52</v>
       </c>
@@ -6630,7 +6633,7 @@
       </c>
     </row>
     <row r="90" spans="1:11">
-      <c r="A90" s="65"/>
+      <c r="A90" s="66"/>
       <c r="B90" s="40" t="s">
         <v>53</v>
       </c>
@@ -6652,7 +6655,7 @@
       <c r="K90" s="13"/>
     </row>
     <row r="91" spans="1:11">
-      <c r="A91" s="65"/>
+      <c r="A91" s="66"/>
       <c r="B91" s="40" t="s">
         <v>190</v>
       </c>
@@ -6756,14 +6759,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="B1" s="66" t="s">
+      <c r="B1" s="67" t="s">
         <v>212</v>
       </c>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
     </row>
     <row r="2" spans="1:7">
       <c r="B2" s="28"/>
@@ -6794,7 +6797,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1">
-      <c r="A4" s="68" t="s">
+      <c r="A4" s="69" t="s">
         <v>37</v>
       </c>
       <c r="B4" s="8" t="s">
@@ -6819,7 +6822,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1">
-      <c r="A5" s="68"/>
+      <c r="A5" s="69"/>
       <c r="B5" s="8" t="s">
         <v>185</v>
       </c>
@@ -6842,7 +6845,7 @@
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="68"/>
+      <c r="A6" s="69"/>
       <c r="B6" s="8" t="s">
         <v>5</v>
       </c>
@@ -6865,7 +6868,7 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="68"/>
+      <c r="A7" s="69"/>
       <c r="B7" s="8" t="s">
         <v>125</v>
       </c>
@@ -6889,7 +6892,7 @@
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="68"/>
+      <c r="A8" s="69"/>
       <c r="B8" s="8" t="s">
         <v>126</v>
       </c>
@@ -6913,7 +6916,7 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="68"/>
+      <c r="A9" s="69"/>
       <c r="B9" s="8" t="s">
         <v>127</v>
       </c>
@@ -6936,7 +6939,7 @@
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="68"/>
+      <c r="A10" s="69"/>
       <c r="B10" s="8" t="s">
         <v>54</v>
       </c>
@@ -6960,7 +6963,7 @@
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="68"/>
+      <c r="A11" s="69"/>
       <c r="B11" s="8" t="s">
         <v>134</v>
       </c>
@@ -6984,7 +6987,7 @@
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="68"/>
+      <c r="A12" s="69"/>
       <c r="B12" s="8" t="s">
         <v>121</v>
       </c>
@@ -7008,7 +7011,7 @@
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="68"/>
+      <c r="A13" s="69"/>
       <c r="B13" s="57" t="s">
         <v>128</v>
       </c>
@@ -7029,7 +7032,7 @@
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="68"/>
+      <c r="A14" s="69"/>
       <c r="B14" s="57" t="s">
         <v>129</v>
       </c>
@@ -7050,7 +7053,7 @@
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="68"/>
+      <c r="A15" s="69"/>
       <c r="B15" s="57" t="s">
         <v>130</v>
       </c>
@@ -7071,7 +7074,7 @@
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="68"/>
+      <c r="A16" s="69"/>
       <c r="B16" s="57" t="s">
         <v>131</v>
       </c>
@@ -7092,7 +7095,7 @@
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="68"/>
+      <c r="A17" s="69"/>
       <c r="B17" s="57" t="s">
         <v>132</v>
       </c>
@@ -7113,7 +7116,7 @@
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="69"/>
+      <c r="A18" s="70"/>
       <c r="B18" s="57" t="s">
         <v>133</v>
       </c>
@@ -7134,7 +7137,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" s="30" customFormat="1" ht="14.7" customHeight="1">
-      <c r="A19" s="70" t="s">
+      <c r="A19" s="71" t="s">
         <v>56</v>
       </c>
       <c r="B19" s="43" t="s">
@@ -7160,7 +7163,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" s="30" customFormat="1">
-      <c r="A20" s="71"/>
+      <c r="A20" s="72"/>
       <c r="B20" s="43" t="s">
         <v>62</v>
       </c>
@@ -7184,7 +7187,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" s="30" customFormat="1">
-      <c r="A21" s="71"/>
+      <c r="A21" s="72"/>
       <c r="B21" s="43" t="s">
         <v>63</v>
       </c>
@@ -7208,7 +7211,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="14.55" customHeight="1">
-      <c r="A22" s="72" t="s">
+      <c r="A22" s="73" t="s">
         <v>58</v>
       </c>
       <c r="B22" s="32" t="s">
@@ -7234,7 +7237,7 @@
       </c>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="73"/>
+      <c r="A23" s="74"/>
       <c r="B23" s="22" t="s">
         <v>64</v>
       </c>
@@ -7258,7 +7261,7 @@
       </c>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="73"/>
+      <c r="A24" s="74"/>
       <c r="B24" s="22" t="s">
         <v>174</v>
       </c>
@@ -7282,7 +7285,7 @@
       </c>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="73"/>
+      <c r="A25" s="74"/>
       <c r="B25" s="22" t="s">
         <v>122</v>
       </c>
@@ -7306,7 +7309,7 @@
       </c>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="73"/>
+      <c r="A26" s="74"/>
       <c r="B26" s="32" t="s">
         <v>175</v>
       </c>
@@ -7329,7 +7332,7 @@
       </c>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="73"/>
+      <c r="A27" s="74"/>
       <c r="B27" s="32" t="s">
         <v>176</v>
       </c>
@@ -7352,7 +7355,7 @@
       </c>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="73"/>
+      <c r="A28" s="74"/>
       <c r="B28" s="22" t="s">
         <v>70</v>
       </c>
@@ -7375,7 +7378,7 @@
       </c>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="73"/>
+      <c r="A29" s="74"/>
       <c r="B29" s="22" t="s">
         <v>71</v>
       </c>
@@ -7398,7 +7401,7 @@
       </c>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="73"/>
+      <c r="A30" s="74"/>
       <c r="B30" s="22" t="s">
         <v>74</v>
       </c>
@@ -7421,7 +7424,7 @@
       </c>
     </row>
     <row r="31" spans="1:7" ht="14.55" customHeight="1">
-      <c r="A31" s="74" t="s">
+      <c r="A31" s="75" t="s">
         <v>34</v>
       </c>
       <c r="B31" s="9" t="s">
@@ -7445,7 +7448,7 @@
       </c>
     </row>
     <row r="32" spans="1:7" ht="14.55" customHeight="1">
-      <c r="A32" s="75"/>
+      <c r="A32" s="76"/>
       <c r="B32" s="9" t="s">
         <v>12</v>
       </c>
@@ -7467,7 +7470,7 @@
       </c>
     </row>
     <row r="33" spans="1:13">
-      <c r="A33" s="75"/>
+      <c r="A33" s="76"/>
       <c r="B33" s="9" t="s">
         <v>142</v>
       </c>
@@ -7489,7 +7492,7 @@
       </c>
     </row>
     <row r="34" spans="1:13">
-      <c r="A34" s="75"/>
+      <c r="A34" s="76"/>
       <c r="B34" s="9" t="s">
         <v>19</v>
       </c>
@@ -7510,7 +7513,7 @@
       </c>
     </row>
     <row r="35" spans="1:13">
-      <c r="A35" s="75"/>
+      <c r="A35" s="76"/>
       <c r="B35" s="9" t="s">
         <v>13</v>
       </c>
@@ -7531,7 +7534,7 @@
       </c>
     </row>
     <row r="36" spans="1:13">
-      <c r="A36" s="75"/>
+      <c r="A36" s="76"/>
       <c r="B36" s="9" t="s">
         <v>14</v>
       </c>
@@ -7552,7 +7555,7 @@
       </c>
     </row>
     <row r="37" spans="1:13">
-      <c r="A37" s="75"/>
+      <c r="A37" s="76"/>
       <c r="B37" s="9" t="s">
         <v>15</v>
       </c>
@@ -7573,7 +7576,7 @@
       </c>
     </row>
     <row r="38" spans="1:13">
-      <c r="A38" s="75"/>
+      <c r="A38" s="76"/>
       <c r="B38" s="9" t="s">
         <v>16</v>
       </c>
@@ -7594,7 +7597,7 @@
       </c>
     </row>
     <row r="39" spans="1:13">
-      <c r="A39" s="75"/>
+      <c r="A39" s="76"/>
       <c r="B39" s="9" t="s">
         <v>146</v>
       </c>
@@ -7615,7 +7618,7 @@
       </c>
     </row>
     <row r="40" spans="1:13">
-      <c r="A40" s="75"/>
+      <c r="A40" s="76"/>
       <c r="B40" s="9" t="s">
         <v>20</v>
       </c>
@@ -7636,7 +7639,7 @@
       </c>
     </row>
     <row r="41" spans="1:13">
-      <c r="A41" s="75"/>
+      <c r="A41" s="76"/>
       <c r="B41" s="9" t="s">
         <v>17</v>
       </c>
@@ -7657,7 +7660,7 @@
       </c>
     </row>
     <row r="42" spans="1:13">
-      <c r="A42" s="75"/>
+      <c r="A42" s="76"/>
       <c r="B42" s="9" t="s">
         <v>18</v>
       </c>
@@ -7678,7 +7681,7 @@
       </c>
     </row>
     <row r="43" spans="1:13" ht="14.55" customHeight="1">
-      <c r="A43" s="76" t="s">
+      <c r="A43" s="77" t="s">
         <v>35</v>
       </c>
       <c r="B43" s="35" t="s">
@@ -7703,7 +7706,7 @@
       </c>
     </row>
     <row r="44" spans="1:13" ht="14.55" customHeight="1">
-      <c r="A44" s="77"/>
+      <c r="A44" s="78"/>
       <c r="B44" s="35" t="s">
         <v>119</v>
       </c>
@@ -7731,7 +7734,7 @@
       <c r="M44" s="51"/>
     </row>
     <row r="45" spans="1:13" ht="14.55" customHeight="1">
-      <c r="A45" s="77"/>
+      <c r="A45" s="78"/>
       <c r="B45" s="35" t="s">
         <v>120</v>
       </c>
@@ -7759,7 +7762,7 @@
       <c r="M45" s="51"/>
     </row>
     <row r="46" spans="1:13" ht="14.55" customHeight="1">
-      <c r="A46" s="77"/>
+      <c r="A46" s="78"/>
       <c r="B46" s="47" t="s">
         <v>194</v>
       </c>
@@ -7789,7 +7792,7 @@
       <c r="M46" s="51"/>
     </row>
     <row r="47" spans="1:13">
-      <c r="A47" s="77"/>
+      <c r="A47" s="78"/>
       <c r="B47" s="35" t="s">
         <v>21</v>
       </c>
@@ -7818,7 +7821,7 @@
       <c r="M47" s="51"/>
     </row>
     <row r="48" spans="1:13">
-      <c r="A48" s="77"/>
+      <c r="A48" s="78"/>
       <c r="B48" s="35" t="s">
         <v>22</v>
       </c>
@@ -7847,7 +7850,7 @@
       <c r="M48" s="51"/>
     </row>
     <row r="49" spans="1:13">
-      <c r="A49" s="77"/>
+      <c r="A49" s="78"/>
       <c r="B49" s="35" t="s">
         <v>23</v>
       </c>
@@ -7876,7 +7879,7 @@
       <c r="M49" s="51"/>
     </row>
     <row r="50" spans="1:13">
-      <c r="A50" s="78"/>
+      <c r="A50" s="79"/>
       <c r="B50" s="35" t="s">
         <v>138</v>
       </c>
@@ -8048,7 +8051,7 @@
       </c>
     </row>
     <row r="57" spans="1:13" ht="14.55" customHeight="1">
-      <c r="A57" s="79" t="s">
+      <c r="A57" s="62" t="s">
         <v>33</v>
       </c>
       <c r="B57" s="17" t="s">
@@ -8075,7 +8078,7 @@
       <c r="K57" s="13"/>
     </row>
     <row r="58" spans="1:13">
-      <c r="A58" s="62"/>
+      <c r="A58" s="63"/>
       <c r="B58" s="17" t="s">
         <v>151</v>
       </c>
@@ -8100,7 +8103,7 @@
       <c r="K58" s="13"/>
     </row>
     <row r="59" spans="1:13">
-      <c r="A59" s="62"/>
+      <c r="A59" s="63"/>
       <c r="B59" s="17" t="s">
         <v>197</v>
       </c>
@@ -8125,7 +8128,7 @@
       <c r="K59" s="13"/>
     </row>
     <row r="60" spans="1:13">
-      <c r="A60" s="62"/>
+      <c r="A60" s="63"/>
       <c r="B60" s="17" t="s">
         <v>198</v>
       </c>
@@ -8146,7 +8149,7 @@
       <c r="K60" s="13"/>
     </row>
     <row r="61" spans="1:13">
-      <c r="A61" s="62"/>
+      <c r="A61" s="63"/>
       <c r="B61" s="17" t="s">
         <v>199</v>
       </c>
@@ -8167,7 +8170,7 @@
       <c r="K61" s="13"/>
     </row>
     <row r="62" spans="1:13">
-      <c r="A62" s="62"/>
+      <c r="A62" s="63"/>
       <c r="B62" s="17" t="s">
         <v>214</v>
       </c>
@@ -8192,7 +8195,7 @@
       <c r="K62" s="13"/>
     </row>
     <row r="63" spans="1:13">
-      <c r="A63" s="62"/>
+      <c r="A63" s="63"/>
       <c r="B63" s="17" t="s">
         <v>155</v>
       </c>
@@ -8217,7 +8220,7 @@
       <c r="K63" s="13"/>
     </row>
     <row r="64" spans="1:13">
-      <c r="A64" s="62"/>
+      <c r="A64" s="63"/>
       <c r="B64" s="20" t="s">
         <v>200</v>
       </c>
@@ -8241,7 +8244,7 @@
       </c>
     </row>
     <row r="65" spans="1:11">
-      <c r="A65" s="62"/>
+      <c r="A65" s="63"/>
       <c r="B65" s="20" t="s">
         <v>201</v>
       </c>
@@ -8261,7 +8264,7 @@
       <c r="G65" s="19"/>
     </row>
     <row r="66" spans="1:11">
-      <c r="A66" s="62"/>
+      <c r="A66" s="63"/>
       <c r="B66" s="20" t="s">
         <v>202</v>
       </c>
@@ -8281,7 +8284,7 @@
       <c r="G66" s="19"/>
     </row>
     <row r="67" spans="1:11">
-      <c r="A67" s="62"/>
+      <c r="A67" s="63"/>
       <c r="B67" s="20" t="s">
         <v>117</v>
       </c>
@@ -8305,7 +8308,7 @@
       <c r="K67" s="13"/>
     </row>
     <row r="68" spans="1:11" ht="14.55" customHeight="1">
-      <c r="A68" s="62"/>
+      <c r="A68" s="63"/>
       <c r="B68" s="20" t="s">
         <v>159</v>
       </c>
@@ -8325,7 +8328,7 @@
       <c r="K68" s="13"/>
     </row>
     <row r="69" spans="1:11" ht="14.55" customHeight="1">
-      <c r="A69" s="62"/>
+      <c r="A69" s="63"/>
       <c r="B69" s="20" t="s">
         <v>206</v>
       </c>
@@ -8349,7 +8352,7 @@
       <c r="K69" s="13"/>
     </row>
     <row r="70" spans="1:11" ht="14.55" customHeight="1">
-      <c r="A70" s="62"/>
+      <c r="A70" s="63"/>
       <c r="B70" s="17" t="s">
         <v>161</v>
       </c>
@@ -8373,7 +8376,7 @@
       <c r="K70" s="13"/>
     </row>
     <row r="71" spans="1:11">
-      <c r="A71" s="62"/>
+      <c r="A71" s="63"/>
       <c r="B71" s="17" t="s">
         <v>162</v>
       </c>
@@ -8397,7 +8400,7 @@
       <c r="K71" s="13"/>
     </row>
     <row r="72" spans="1:11">
-      <c r="A72" s="62"/>
+      <c r="A72" s="63"/>
       <c r="B72" s="17" t="s">
         <v>164</v>
       </c>
@@ -8421,7 +8424,7 @@
       <c r="K72" s="13"/>
     </row>
     <row r="73" spans="1:11">
-      <c r="A73" s="63"/>
+      <c r="A73" s="64"/>
       <c r="B73" s="17" t="s">
         <v>76</v>
       </c>
@@ -8445,7 +8448,7 @@
       <c r="K73" s="13"/>
     </row>
     <row r="74" spans="1:11" ht="14.55" customHeight="1">
-      <c r="A74" s="64" t="s">
+      <c r="A74" s="65" t="s">
         <v>38</v>
       </c>
       <c r="B74" s="40" t="s">
@@ -8468,7 +8471,7 @@
       </c>
     </row>
     <row r="75" spans="1:11">
-      <c r="A75" s="65"/>
+      <c r="A75" s="66"/>
       <c r="B75" s="40" t="s">
         <v>48</v>
       </c>
@@ -8489,7 +8492,7 @@
       </c>
     </row>
     <row r="76" spans="1:11">
-      <c r="A76" s="65"/>
+      <c r="A76" s="66"/>
       <c r="B76" s="40" t="s">
         <v>40</v>
       </c>
@@ -8510,7 +8513,7 @@
       </c>
     </row>
     <row r="77" spans="1:11">
-      <c r="A77" s="65"/>
+      <c r="A77" s="66"/>
       <c r="B77" s="40" t="s">
         <v>41</v>
       </c>
@@ -8531,7 +8534,7 @@
       </c>
     </row>
     <row r="78" spans="1:11">
-      <c r="A78" s="65"/>
+      <c r="A78" s="66"/>
       <c r="B78" s="40" t="s">
         <v>42</v>
       </c>
@@ -8552,7 +8555,7 @@
       </c>
     </row>
     <row r="79" spans="1:11">
-      <c r="A79" s="65"/>
+      <c r="A79" s="66"/>
       <c r="B79" s="40" t="s">
         <v>188</v>
       </c>
@@ -8574,7 +8577,7 @@
       <c r="K79" s="13"/>
     </row>
     <row r="80" spans="1:11">
-      <c r="A80" s="65"/>
+      <c r="A80" s="66"/>
       <c r="B80" s="40" t="s">
         <v>43</v>
       </c>
@@ -8596,7 +8599,7 @@
       <c r="K80" s="13"/>
     </row>
     <row r="81" spans="1:11">
-      <c r="A81" s="65"/>
+      <c r="A81" s="66"/>
       <c r="B81" s="40" t="s">
         <v>49</v>
       </c>
@@ -8618,7 +8621,7 @@
       <c r="K81" s="13"/>
     </row>
     <row r="82" spans="1:11">
-      <c r="A82" s="65"/>
+      <c r="A82" s="66"/>
       <c r="B82" s="40" t="s">
         <v>44</v>
       </c>
@@ -8640,7 +8643,7 @@
       <c r="K82" s="13"/>
     </row>
     <row r="83" spans="1:11">
-      <c r="A83" s="65"/>
+      <c r="A83" s="66"/>
       <c r="B83" s="40" t="s">
         <v>45</v>
       </c>
@@ -8662,7 +8665,7 @@
       <c r="K83" s="13"/>
     </row>
     <row r="84" spans="1:11">
-      <c r="A84" s="65"/>
+      <c r="A84" s="66"/>
       <c r="B84" s="40" t="s">
         <v>46</v>
       </c>
@@ -8683,7 +8686,7 @@
       </c>
     </row>
     <row r="85" spans="1:11">
-      <c r="A85" s="65"/>
+      <c r="A85" s="66"/>
       <c r="B85" s="40" t="s">
         <v>189</v>
       </c>
@@ -8704,7 +8707,7 @@
       </c>
     </row>
     <row r="86" spans="1:11">
-      <c r="A86" s="65"/>
+      <c r="A86" s="66"/>
       <c r="B86" s="40" t="s">
         <v>47</v>
       </c>
@@ -8725,7 +8728,7 @@
       </c>
     </row>
     <row r="87" spans="1:11">
-      <c r="A87" s="65"/>
+      <c r="A87" s="66"/>
       <c r="B87" s="40" t="s">
         <v>50</v>
       </c>
@@ -8746,7 +8749,7 @@
       </c>
     </row>
     <row r="88" spans="1:11">
-      <c r="A88" s="65"/>
+      <c r="A88" s="66"/>
       <c r="B88" s="40" t="s">
         <v>51</v>
       </c>
@@ -8767,7 +8770,7 @@
       </c>
     </row>
     <row r="89" spans="1:11">
-      <c r="A89" s="65"/>
+      <c r="A89" s="66"/>
       <c r="B89" s="40" t="s">
         <v>52</v>
       </c>
@@ -8788,7 +8791,7 @@
       </c>
     </row>
     <row r="90" spans="1:11">
-      <c r="A90" s="65"/>
+      <c r="A90" s="66"/>
       <c r="B90" s="40" t="s">
         <v>53</v>
       </c>
@@ -8810,7 +8813,7 @@
       <c r="K90" s="13"/>
     </row>
     <row r="91" spans="1:11">
-      <c r="A91" s="65"/>
+      <c r="A91" s="66"/>
       <c r="B91" s="40" t="s">
         <v>190</v>
       </c>
@@ -8914,14 +8917,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="B1" s="66" t="s">
+      <c r="B1" s="67" t="s">
         <v>212</v>
       </c>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
     </row>
     <row r="2" spans="1:7">
       <c r="B2" s="28"/>
@@ -8952,7 +8955,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1">
-      <c r="A4" s="68" t="s">
+      <c r="A4" s="69" t="s">
         <v>37</v>
       </c>
       <c r="B4" s="8" t="s">
@@ -8977,7 +8980,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1">
-      <c r="A5" s="68"/>
+      <c r="A5" s="69"/>
       <c r="B5" s="8" t="s">
         <v>185</v>
       </c>
@@ -9000,7 +9003,7 @@
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="68"/>
+      <c r="A6" s="69"/>
       <c r="B6" s="8" t="s">
         <v>5</v>
       </c>
@@ -9023,7 +9026,7 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="68"/>
+      <c r="A7" s="69"/>
       <c r="B7" s="8" t="s">
         <v>125</v>
       </c>
@@ -9046,7 +9049,7 @@
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="68"/>
+      <c r="A8" s="69"/>
       <c r="B8" s="8" t="s">
         <v>126</v>
       </c>
@@ -9070,7 +9073,7 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="68"/>
+      <c r="A9" s="69"/>
       <c r="B9" s="8" t="s">
         <v>127</v>
       </c>
@@ -9093,7 +9096,7 @@
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="68"/>
+      <c r="A10" s="69"/>
       <c r="B10" s="8" t="s">
         <v>54</v>
       </c>
@@ -9117,7 +9120,7 @@
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="68"/>
+      <c r="A11" s="69"/>
       <c r="B11" s="8" t="s">
         <v>134</v>
       </c>
@@ -9141,7 +9144,7 @@
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="68"/>
+      <c r="A12" s="69"/>
       <c r="B12" s="8" t="s">
         <v>121</v>
       </c>
@@ -9165,7 +9168,7 @@
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="68"/>
+      <c r="A13" s="69"/>
       <c r="B13" s="8" t="s">
         <v>128</v>
       </c>
@@ -9186,7 +9189,7 @@
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="68"/>
+      <c r="A14" s="69"/>
       <c r="B14" s="8" t="s">
         <v>129</v>
       </c>
@@ -9207,7 +9210,7 @@
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="68"/>
+      <c r="A15" s="69"/>
       <c r="B15" s="8" t="s">
         <v>130</v>
       </c>
@@ -9228,7 +9231,7 @@
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="68"/>
+      <c r="A16" s="69"/>
       <c r="B16" s="8" t="s">
         <v>131</v>
       </c>
@@ -9249,7 +9252,7 @@
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="68"/>
+      <c r="A17" s="69"/>
       <c r="B17" s="8" t="s">
         <v>132</v>
       </c>
@@ -9270,7 +9273,7 @@
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="69"/>
+      <c r="A18" s="70"/>
       <c r="B18" s="8" t="s">
         <v>133</v>
       </c>
@@ -9291,7 +9294,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" s="30" customFormat="1" ht="14.7" customHeight="1">
-      <c r="A19" s="70" t="s">
+      <c r="A19" s="71" t="s">
         <v>56</v>
       </c>
       <c r="B19" s="43" t="s">
@@ -9317,7 +9320,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" s="30" customFormat="1">
-      <c r="A20" s="71"/>
+      <c r="A20" s="72"/>
       <c r="B20" s="43" t="s">
         <v>62</v>
       </c>
@@ -9341,7 +9344,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" s="30" customFormat="1">
-      <c r="A21" s="71"/>
+      <c r="A21" s="72"/>
       <c r="B21" s="43" t="s">
         <v>63</v>
       </c>
@@ -9365,7 +9368,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="14.55" customHeight="1">
-      <c r="A22" s="72" t="s">
+      <c r="A22" s="73" t="s">
         <v>58</v>
       </c>
       <c r="B22" s="32" t="s">
@@ -9391,7 +9394,7 @@
       </c>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="73"/>
+      <c r="A23" s="74"/>
       <c r="B23" s="22" t="s">
         <v>64</v>
       </c>
@@ -9415,7 +9418,7 @@
       </c>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="73"/>
+      <c r="A24" s="74"/>
       <c r="B24" s="22" t="s">
         <v>174</v>
       </c>
@@ -9439,7 +9442,7 @@
       </c>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="73"/>
+      <c r="A25" s="74"/>
       <c r="B25" s="22" t="s">
         <v>122</v>
       </c>
@@ -9463,7 +9466,7 @@
       </c>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="73"/>
+      <c r="A26" s="74"/>
       <c r="B26" s="32" t="s">
         <v>175</v>
       </c>
@@ -9486,7 +9489,7 @@
       </c>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="73"/>
+      <c r="A27" s="74"/>
       <c r="B27" s="32" t="s">
         <v>176</v>
       </c>
@@ -9509,7 +9512,7 @@
       </c>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="73"/>
+      <c r="A28" s="74"/>
       <c r="B28" s="22" t="s">
         <v>70</v>
       </c>
@@ -9532,7 +9535,7 @@
       </c>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="73"/>
+      <c r="A29" s="74"/>
       <c r="B29" s="22" t="s">
         <v>71</v>
       </c>
@@ -9555,7 +9558,7 @@
       </c>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="73"/>
+      <c r="A30" s="74"/>
       <c r="B30" s="22" t="s">
         <v>74</v>
       </c>
@@ -9578,7 +9581,7 @@
       </c>
     </row>
     <row r="31" spans="1:7" ht="14.55" customHeight="1">
-      <c r="A31" s="74" t="s">
+      <c r="A31" s="75" t="s">
         <v>34</v>
       </c>
       <c r="B31" s="9" t="s">
@@ -9602,7 +9605,7 @@
       </c>
     </row>
     <row r="32" spans="1:7" ht="14.55" customHeight="1">
-      <c r="A32" s="75"/>
+      <c r="A32" s="76"/>
       <c r="B32" s="9" t="s">
         <v>12</v>
       </c>
@@ -9624,7 +9627,7 @@
       </c>
     </row>
     <row r="33" spans="1:13">
-      <c r="A33" s="75"/>
+      <c r="A33" s="76"/>
       <c r="B33" s="9" t="s">
         <v>142</v>
       </c>
@@ -9646,7 +9649,7 @@
       </c>
     </row>
     <row r="34" spans="1:13">
-      <c r="A34" s="75"/>
+      <c r="A34" s="76"/>
       <c r="B34" s="9" t="s">
         <v>19</v>
       </c>
@@ -9667,7 +9670,7 @@
       </c>
     </row>
     <row r="35" spans="1:13">
-      <c r="A35" s="75"/>
+      <c r="A35" s="76"/>
       <c r="B35" s="9" t="s">
         <v>13</v>
       </c>
@@ -9688,7 +9691,7 @@
       </c>
     </row>
     <row r="36" spans="1:13">
-      <c r="A36" s="75"/>
+      <c r="A36" s="76"/>
       <c r="B36" s="9" t="s">
         <v>14</v>
       </c>
@@ -9709,7 +9712,7 @@
       </c>
     </row>
     <row r="37" spans="1:13">
-      <c r="A37" s="75"/>
+      <c r="A37" s="76"/>
       <c r="B37" s="9" t="s">
         <v>15</v>
       </c>
@@ -9730,7 +9733,7 @@
       </c>
     </row>
     <row r="38" spans="1:13">
-      <c r="A38" s="75"/>
+      <c r="A38" s="76"/>
       <c r="B38" s="9" t="s">
         <v>16</v>
       </c>
@@ -9751,7 +9754,7 @@
       </c>
     </row>
     <row r="39" spans="1:13">
-      <c r="A39" s="75"/>
+      <c r="A39" s="76"/>
       <c r="B39" s="9" t="s">
         <v>146</v>
       </c>
@@ -9772,7 +9775,7 @@
       </c>
     </row>
     <row r="40" spans="1:13">
-      <c r="A40" s="75"/>
+      <c r="A40" s="76"/>
       <c r="B40" s="9" t="s">
         <v>20</v>
       </c>
@@ -9793,7 +9796,7 @@
       </c>
     </row>
     <row r="41" spans="1:13">
-      <c r="A41" s="75"/>
+      <c r="A41" s="76"/>
       <c r="B41" s="9" t="s">
         <v>17</v>
       </c>
@@ -9814,7 +9817,7 @@
       </c>
     </row>
     <row r="42" spans="1:13">
-      <c r="A42" s="75"/>
+      <c r="A42" s="76"/>
       <c r="B42" s="9" t="s">
         <v>18</v>
       </c>
@@ -9835,7 +9838,7 @@
       </c>
     </row>
     <row r="43" spans="1:13" ht="14.55" customHeight="1">
-      <c r="A43" s="76" t="s">
+      <c r="A43" s="77" t="s">
         <v>35</v>
       </c>
       <c r="B43" s="35" t="s">
@@ -9860,7 +9863,7 @@
       </c>
     </row>
     <row r="44" spans="1:13" ht="14.55" customHeight="1">
-      <c r="A44" s="77"/>
+      <c r="A44" s="78"/>
       <c r="B44" s="35" t="s">
         <v>119</v>
       </c>
@@ -9888,7 +9891,7 @@
       <c r="M44" s="51"/>
     </row>
     <row r="45" spans="1:13" ht="14.55" customHeight="1">
-      <c r="A45" s="77"/>
+      <c r="A45" s="78"/>
       <c r="B45" s="35" t="s">
         <v>120</v>
       </c>
@@ -9916,7 +9919,7 @@
       <c r="M45" s="51"/>
     </row>
     <row r="46" spans="1:13" ht="14.55" customHeight="1">
-      <c r="A46" s="77"/>
+      <c r="A46" s="78"/>
       <c r="B46" s="47" t="s">
         <v>194</v>
       </c>
@@ -9946,7 +9949,7 @@
       <c r="M46" s="51"/>
     </row>
     <row r="47" spans="1:13">
-      <c r="A47" s="77"/>
+      <c r="A47" s="78"/>
       <c r="B47" s="35" t="s">
         <v>21</v>
       </c>
@@ -9975,7 +9978,7 @@
       <c r="M47" s="51"/>
     </row>
     <row r="48" spans="1:13">
-      <c r="A48" s="77"/>
+      <c r="A48" s="78"/>
       <c r="B48" s="35" t="s">
         <v>22</v>
       </c>
@@ -10004,7 +10007,7 @@
       <c r="M48" s="51"/>
     </row>
     <row r="49" spans="1:13">
-      <c r="A49" s="77"/>
+      <c r="A49" s="78"/>
       <c r="B49" s="35" t="s">
         <v>23</v>
       </c>
@@ -10033,7 +10036,7 @@
       <c r="M49" s="51"/>
     </row>
     <row r="50" spans="1:13">
-      <c r="A50" s="78"/>
+      <c r="A50" s="79"/>
       <c r="B50" s="35" t="s">
         <v>138</v>
       </c>
@@ -10205,7 +10208,7 @@
       </c>
     </row>
     <row r="57" spans="1:13" ht="14.55" customHeight="1">
-      <c r="A57" s="79" t="s">
+      <c r="A57" s="62" t="s">
         <v>33</v>
       </c>
       <c r="B57" s="17" t="s">
@@ -10232,7 +10235,7 @@
       <c r="K57" s="13"/>
     </row>
     <row r="58" spans="1:13">
-      <c r="A58" s="62"/>
+      <c r="A58" s="63"/>
       <c r="B58" s="17" t="s">
         <v>151</v>
       </c>
@@ -10257,7 +10260,7 @@
       <c r="K58" s="13"/>
     </row>
     <row r="59" spans="1:13">
-      <c r="A59" s="62"/>
+      <c r="A59" s="63"/>
       <c r="B59" s="17" t="s">
         <v>197</v>
       </c>
@@ -10282,7 +10285,7 @@
       <c r="K59" s="13"/>
     </row>
     <row r="60" spans="1:13">
-      <c r="A60" s="62"/>
+      <c r="A60" s="63"/>
       <c r="B60" s="17" t="s">
         <v>198</v>
       </c>
@@ -10303,7 +10306,7 @@
       <c r="K60" s="13"/>
     </row>
     <row r="61" spans="1:13">
-      <c r="A61" s="62"/>
+      <c r="A61" s="63"/>
       <c r="B61" s="17" t="s">
         <v>199</v>
       </c>
@@ -10324,7 +10327,7 @@
       <c r="K61" s="13"/>
     </row>
     <row r="62" spans="1:13">
-      <c r="A62" s="62"/>
+      <c r="A62" s="63"/>
       <c r="B62" s="17" t="s">
         <v>214</v>
       </c>
@@ -10349,7 +10352,7 @@
       <c r="K62" s="13"/>
     </row>
     <row r="63" spans="1:13">
-      <c r="A63" s="62"/>
+      <c r="A63" s="63"/>
       <c r="B63" s="17" t="s">
         <v>155</v>
       </c>
@@ -10374,7 +10377,7 @@
       <c r="K63" s="13"/>
     </row>
     <row r="64" spans="1:13">
-      <c r="A64" s="62"/>
+      <c r="A64" s="63"/>
       <c r="B64" s="20" t="s">
         <v>200</v>
       </c>
@@ -10398,7 +10401,7 @@
       </c>
     </row>
     <row r="65" spans="1:11">
-      <c r="A65" s="62"/>
+      <c r="A65" s="63"/>
       <c r="B65" s="20" t="s">
         <v>201</v>
       </c>
@@ -10418,7 +10421,7 @@
       <c r="G65" s="19"/>
     </row>
     <row r="66" spans="1:11">
-      <c r="A66" s="62"/>
+      <c r="A66" s="63"/>
       <c r="B66" s="20" t="s">
         <v>202</v>
       </c>
@@ -10438,7 +10441,7 @@
       <c r="G66" s="19"/>
     </row>
     <row r="67" spans="1:11">
-      <c r="A67" s="62"/>
+      <c r="A67" s="63"/>
       <c r="B67" s="20" t="s">
         <v>117</v>
       </c>
@@ -10462,7 +10465,7 @@
       <c r="K67" s="13"/>
     </row>
     <row r="68" spans="1:11" ht="14.55" customHeight="1">
-      <c r="A68" s="62"/>
+      <c r="A68" s="63"/>
       <c r="B68" s="20" t="s">
         <v>159</v>
       </c>
@@ -10483,7 +10486,7 @@
       <c r="K68" s="13"/>
     </row>
     <row r="69" spans="1:11" ht="14.55" customHeight="1">
-      <c r="A69" s="62"/>
+      <c r="A69" s="63"/>
       <c r="B69" s="20" t="s">
         <v>206</v>
       </c>
@@ -10507,7 +10510,7 @@
       <c r="K69" s="13"/>
     </row>
     <row r="70" spans="1:11" ht="14.55" customHeight="1">
-      <c r="A70" s="62"/>
+      <c r="A70" s="63"/>
       <c r="B70" s="17" t="s">
         <v>161</v>
       </c>
@@ -10531,7 +10534,7 @@
       <c r="K70" s="13"/>
     </row>
     <row r="71" spans="1:11">
-      <c r="A71" s="62"/>
+      <c r="A71" s="63"/>
       <c r="B71" s="17" t="s">
         <v>162</v>
       </c>
@@ -10555,7 +10558,7 @@
       <c r="K71" s="13"/>
     </row>
     <row r="72" spans="1:11">
-      <c r="A72" s="62"/>
+      <c r="A72" s="63"/>
       <c r="B72" s="17" t="s">
         <v>164</v>
       </c>
@@ -10579,7 +10582,7 @@
       <c r="K72" s="13"/>
     </row>
     <row r="73" spans="1:11">
-      <c r="A73" s="63"/>
+      <c r="A73" s="64"/>
       <c r="B73" s="17" t="s">
         <v>76</v>
       </c>
@@ -10603,7 +10606,7 @@
       <c r="K73" s="13"/>
     </row>
     <row r="74" spans="1:11" ht="14.55" customHeight="1">
-      <c r="A74" s="64" t="s">
+      <c r="A74" s="65" t="s">
         <v>38</v>
       </c>
       <c r="B74" s="40" t="s">
@@ -10626,7 +10629,7 @@
       </c>
     </row>
     <row r="75" spans="1:11">
-      <c r="A75" s="65"/>
+      <c r="A75" s="66"/>
       <c r="B75" s="40" t="s">
         <v>48</v>
       </c>
@@ -10647,7 +10650,7 @@
       </c>
     </row>
     <row r="76" spans="1:11">
-      <c r="A76" s="65"/>
+      <c r="A76" s="66"/>
       <c r="B76" s="40" t="s">
         <v>40</v>
       </c>
@@ -10668,7 +10671,7 @@
       </c>
     </row>
     <row r="77" spans="1:11">
-      <c r="A77" s="65"/>
+      <c r="A77" s="66"/>
       <c r="B77" s="40" t="s">
         <v>41</v>
       </c>
@@ -10689,7 +10692,7 @@
       </c>
     </row>
     <row r="78" spans="1:11">
-      <c r="A78" s="65"/>
+      <c r="A78" s="66"/>
       <c r="B78" s="40" t="s">
         <v>42</v>
       </c>
@@ -10710,7 +10713,7 @@
       </c>
     </row>
     <row r="79" spans="1:11">
-      <c r="A79" s="65"/>
+      <c r="A79" s="66"/>
       <c r="B79" s="40" t="s">
         <v>188</v>
       </c>
@@ -10732,7 +10735,7 @@
       <c r="K79" s="13"/>
     </row>
     <row r="80" spans="1:11">
-      <c r="A80" s="65"/>
+      <c r="A80" s="66"/>
       <c r="B80" s="40" t="s">
         <v>43</v>
       </c>
@@ -10754,7 +10757,7 @@
       <c r="K80" s="13"/>
     </row>
     <row r="81" spans="1:11">
-      <c r="A81" s="65"/>
+      <c r="A81" s="66"/>
       <c r="B81" s="40" t="s">
         <v>49</v>
       </c>
@@ -10776,7 +10779,7 @@
       <c r="K81" s="13"/>
     </row>
     <row r="82" spans="1:11">
-      <c r="A82" s="65"/>
+      <c r="A82" s="66"/>
       <c r="B82" s="40" t="s">
         <v>44</v>
       </c>
@@ -10798,7 +10801,7 @@
       <c r="K82" s="13"/>
     </row>
     <row r="83" spans="1:11">
-      <c r="A83" s="65"/>
+      <c r="A83" s="66"/>
       <c r="B83" s="40" t="s">
         <v>45</v>
       </c>
@@ -10820,7 +10823,7 @@
       <c r="K83" s="13"/>
     </row>
     <row r="84" spans="1:11">
-      <c r="A84" s="65"/>
+      <c r="A84" s="66"/>
       <c r="B84" s="40" t="s">
         <v>46</v>
       </c>
@@ -10841,7 +10844,7 @@
       </c>
     </row>
     <row r="85" spans="1:11">
-      <c r="A85" s="65"/>
+      <c r="A85" s="66"/>
       <c r="B85" s="40" t="s">
         <v>189</v>
       </c>
@@ -10862,7 +10865,7 @@
       </c>
     </row>
     <row r="86" spans="1:11">
-      <c r="A86" s="65"/>
+      <c r="A86" s="66"/>
       <c r="B86" s="40" t="s">
         <v>47</v>
       </c>
@@ -10883,7 +10886,7 @@
       </c>
     </row>
     <row r="87" spans="1:11">
-      <c r="A87" s="65"/>
+      <c r="A87" s="66"/>
       <c r="B87" s="40" t="s">
         <v>50</v>
       </c>
@@ -10904,7 +10907,7 @@
       </c>
     </row>
     <row r="88" spans="1:11">
-      <c r="A88" s="65"/>
+      <c r="A88" s="66"/>
       <c r="B88" s="40" t="s">
         <v>51</v>
       </c>
@@ -10925,7 +10928,7 @@
       </c>
     </row>
     <row r="89" spans="1:11">
-      <c r="A89" s="65"/>
+      <c r="A89" s="66"/>
       <c r="B89" s="40" t="s">
         <v>52</v>
       </c>
@@ -10946,7 +10949,7 @@
       </c>
     </row>
     <row r="90" spans="1:11">
-      <c r="A90" s="65"/>
+      <c r="A90" s="66"/>
       <c r="B90" s="40" t="s">
         <v>53</v>
       </c>
@@ -10968,7 +10971,7 @@
       <c r="K90" s="13"/>
     </row>
     <row r="91" spans="1:11">
-      <c r="A91" s="65"/>
+      <c r="A91" s="66"/>
       <c r="B91" s="40" t="s">
         <v>190</v>
       </c>
@@ -11055,9 +11058,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D772B5C0-78A8-4453-9C12-C71D4E986150}">
   <dimension ref="A1:M139"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B64" sqref="B64"/>
+      <selection pane="bottomLeft" activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -11069,19 +11072,20 @@
     <col min="5" max="5" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="75.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="B1" s="66" t="s">
+    <row r="1" spans="1:10">
+      <c r="B1" s="67" t="s">
         <v>212</v>
       </c>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+    </row>
+    <row r="2" spans="1:10">
       <c r="B2" s="28"/>
       <c r="C2" s="29"/>
       <c r="D2" s="29"/>
@@ -11089,7 +11093,7 @@
       <c r="F2" s="29"/>
       <c r="G2" s="29"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:10">
       <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
@@ -11109,8 +11113,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15" customHeight="1">
-      <c r="A4" s="68" t="s">
+    <row r="4" spans="1:10" ht="15" customHeight="1">
+      <c r="A4" s="69" t="s">
         <v>37</v>
       </c>
       <c r="B4" s="8" t="s">
@@ -11134,8 +11138,8 @@
         <v>186</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15" customHeight="1">
-      <c r="A5" s="68"/>
+    <row r="5" spans="1:10" ht="15" customHeight="1">
+      <c r="A5" s="69"/>
       <c r="B5" s="8" t="s">
         <v>185</v>
       </c>
@@ -11157,8 +11161,8 @@
         <v>187</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="68"/>
+    <row r="6" spans="1:10">
+      <c r="A6" s="69"/>
       <c r="B6" s="8" t="s">
         <v>5</v>
       </c>
@@ -11180,8 +11184,8 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="68"/>
+    <row r="7" spans="1:10">
+      <c r="A7" s="69"/>
       <c r="B7" s="8" t="s">
         <v>237</v>
       </c>
@@ -11204,8 +11208,8 @@
         <v>183</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="68"/>
+    <row r="8" spans="1:10">
+      <c r="A8" s="69"/>
       <c r="B8" s="8" t="s">
         <v>238</v>
       </c>
@@ -11227,9 +11231,17 @@
       <c r="G8" s="3" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="68"/>
+      <c r="I8">
+        <f>C7*C8*C9*C13</f>
+        <v>2099587.2000000002</v>
+      </c>
+      <c r="J8">
+        <f>I8+I9</f>
+        <v>2172546.3326000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="69"/>
       <c r="B9" s="8" t="s">
         <v>239</v>
       </c>
@@ -11250,9 +11262,13 @@
       <c r="G9" s="3" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="68"/>
+      <c r="I9">
+        <f>C10*C11*C12*C13</f>
+        <v>72959.132599999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="69"/>
       <c r="B10" s="8" t="s">
         <v>240</v>
       </c>
@@ -11274,8 +11290,8 @@
         <v>183</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="68"/>
+    <row r="11" spans="1:10">
+      <c r="A11" s="69"/>
       <c r="B11" s="8" t="s">
         <v>241</v>
       </c>
@@ -11298,8 +11314,8 @@
         <v>182</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="68"/>
+    <row r="12" spans="1:10">
+      <c r="A12" s="69"/>
       <c r="B12" s="8" t="s">
         <v>242</v>
       </c>
@@ -11321,8 +11337,8 @@
         <v>137</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="68"/>
+    <row r="13" spans="1:10">
+      <c r="A13" s="69"/>
       <c r="B13" s="8" t="s">
         <v>54</v>
       </c>
@@ -11345,8 +11361,8 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="68"/>
+    <row r="14" spans="1:10">
+      <c r="A14" s="69"/>
       <c r="B14" s="8" t="s">
         <v>134</v>
       </c>
@@ -11369,8 +11385,8 @@
         <v>172</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="68"/>
+    <row r="15" spans="1:10">
+      <c r="A15" s="69"/>
       <c r="B15" s="8" t="s">
         <v>121</v>
       </c>
@@ -11393,8 +11409,8 @@
         <v>211</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="68"/>
+    <row r="16" spans="1:10">
+      <c r="A16" s="69"/>
       <c r="B16" s="57" t="s">
         <v>128</v>
       </c>
@@ -11415,7 +11431,7 @@
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="68"/>
+      <c r="A17" s="69"/>
       <c r="B17" s="57" t="s">
         <v>129</v>
       </c>
@@ -11436,7 +11452,7 @@
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="68"/>
+      <c r="A18" s="69"/>
       <c r="B18" s="57" t="s">
         <v>130</v>
       </c>
@@ -11457,7 +11473,7 @@
       </c>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="68"/>
+      <c r="A19" s="69"/>
       <c r="B19" s="57" t="s">
         <v>131</v>
       </c>
@@ -11478,7 +11494,7 @@
       </c>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="68"/>
+      <c r="A20" s="69"/>
       <c r="B20" s="57" t="s">
         <v>132</v>
       </c>
@@ -11499,7 +11515,7 @@
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="69"/>
+      <c r="A21" s="70"/>
       <c r="B21" s="57" t="s">
         <v>133</v>
       </c>
@@ -11520,7 +11536,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" s="30" customFormat="1" ht="14.7" customHeight="1">
-      <c r="A22" s="70" t="s">
+      <c r="A22" s="71" t="s">
         <v>56</v>
       </c>
       <c r="B22" s="43" t="s">
@@ -11546,7 +11562,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" s="30" customFormat="1">
-      <c r="A23" s="71"/>
+      <c r="A23" s="72"/>
       <c r="B23" s="43" t="s">
         <v>62</v>
       </c>
@@ -11570,7 +11586,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" s="30" customFormat="1">
-      <c r="A24" s="71"/>
+      <c r="A24" s="72"/>
       <c r="B24" s="43" t="s">
         <v>63</v>
       </c>
@@ -11594,7 +11610,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" ht="14.55" customHeight="1">
-      <c r="A25" s="72" t="s">
+      <c r="A25" s="73" t="s">
         <v>58</v>
       </c>
       <c r="B25" s="32" t="s">
@@ -11620,7 +11636,7 @@
       </c>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="73"/>
+      <c r="A26" s="74"/>
       <c r="B26" s="22" t="s">
         <v>64</v>
       </c>
@@ -11644,7 +11660,7 @@
       </c>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="73"/>
+      <c r="A27" s="74"/>
       <c r="B27" s="22" t="s">
         <v>174</v>
       </c>
@@ -11668,7 +11684,7 @@
       </c>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="73"/>
+      <c r="A28" s="74"/>
       <c r="B28" s="22" t="s">
         <v>122</v>
       </c>
@@ -11692,7 +11708,7 @@
       </c>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="73"/>
+      <c r="A29" s="74"/>
       <c r="B29" s="32" t="s">
         <v>175</v>
       </c>
@@ -11715,7 +11731,7 @@
       </c>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="73"/>
+      <c r="A30" s="74"/>
       <c r="B30" s="32" t="s">
         <v>176</v>
       </c>
@@ -11738,7 +11754,7 @@
       </c>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="73"/>
+      <c r="A31" s="74"/>
       <c r="B31" s="22" t="s">
         <v>70</v>
       </c>
@@ -11761,7 +11777,7 @@
       </c>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="73"/>
+      <c r="A32" s="74"/>
       <c r="B32" s="22" t="s">
         <v>71</v>
       </c>
@@ -11784,7 +11800,7 @@
       </c>
     </row>
     <row r="33" spans="1:13">
-      <c r="A33" s="73"/>
+      <c r="A33" s="74"/>
       <c r="B33" s="22" t="s">
         <v>74</v>
       </c>
@@ -11807,7 +11823,7 @@
       </c>
     </row>
     <row r="34" spans="1:13" ht="14.55" customHeight="1">
-      <c r="A34" s="74" t="s">
+      <c r="A34" s="75" t="s">
         <v>34</v>
       </c>
       <c r="B34" s="9" t="s">
@@ -11831,7 +11847,7 @@
       </c>
     </row>
     <row r="35" spans="1:13" ht="14.55" customHeight="1">
-      <c r="A35" s="75"/>
+      <c r="A35" s="76"/>
       <c r="B35" s="9" t="s">
         <v>12</v>
       </c>
@@ -11853,7 +11869,7 @@
       </c>
     </row>
     <row r="36" spans="1:13">
-      <c r="A36" s="75"/>
+      <c r="A36" s="76"/>
       <c r="B36" s="9" t="s">
         <v>142</v>
       </c>
@@ -11875,7 +11891,7 @@
       </c>
     </row>
     <row r="37" spans="1:13">
-      <c r="A37" s="75"/>
+      <c r="A37" s="76"/>
       <c r="B37" s="9" t="s">
         <v>19</v>
       </c>
@@ -11896,7 +11912,7 @@
       </c>
     </row>
     <row r="38" spans="1:13">
-      <c r="A38" s="75"/>
+      <c r="A38" s="76"/>
       <c r="B38" s="9" t="s">
         <v>13</v>
       </c>
@@ -11917,7 +11933,7 @@
       </c>
     </row>
     <row r="39" spans="1:13">
-      <c r="A39" s="75"/>
+      <c r="A39" s="76"/>
       <c r="B39" s="9" t="s">
         <v>14</v>
       </c>
@@ -11938,7 +11954,7 @@
       </c>
     </row>
     <row r="40" spans="1:13">
-      <c r="A40" s="75"/>
+      <c r="A40" s="76"/>
       <c r="B40" s="9" t="s">
         <v>15</v>
       </c>
@@ -11959,7 +11975,7 @@
       </c>
     </row>
     <row r="41" spans="1:13">
-      <c r="A41" s="75"/>
+      <c r="A41" s="76"/>
       <c r="B41" s="9" t="s">
         <v>16</v>
       </c>
@@ -11980,7 +11996,7 @@
       </c>
     </row>
     <row r="42" spans="1:13">
-      <c r="A42" s="75"/>
+      <c r="A42" s="76"/>
       <c r="B42" s="9" t="s">
         <v>146</v>
       </c>
@@ -12001,7 +12017,7 @@
       </c>
     </row>
     <row r="43" spans="1:13">
-      <c r="A43" s="75"/>
+      <c r="A43" s="76"/>
       <c r="B43" s="9" t="s">
         <v>20</v>
       </c>
@@ -12022,7 +12038,7 @@
       </c>
     </row>
     <row r="44" spans="1:13">
-      <c r="A44" s="75"/>
+      <c r="A44" s="76"/>
       <c r="B44" s="9" t="s">
         <v>17</v>
       </c>
@@ -12043,7 +12059,7 @@
       </c>
     </row>
     <row r="45" spans="1:13">
-      <c r="A45" s="75"/>
+      <c r="A45" s="76"/>
       <c r="B45" s="9" t="s">
         <v>18</v>
       </c>
@@ -12064,7 +12080,7 @@
       </c>
     </row>
     <row r="46" spans="1:13" ht="14.55" customHeight="1">
-      <c r="A46" s="76" t="s">
+      <c r="A46" s="77" t="s">
         <v>35</v>
       </c>
       <c r="B46" s="35" t="s">
@@ -12089,7 +12105,7 @@
       </c>
     </row>
     <row r="47" spans="1:13" ht="14.55" customHeight="1">
-      <c r="A47" s="77"/>
+      <c r="A47" s="78"/>
       <c r="B47" s="35" t="s">
         <v>119</v>
       </c>
@@ -12117,7 +12133,7 @@
       <c r="M47" s="51"/>
     </row>
     <row r="48" spans="1:13" ht="14.55" customHeight="1">
-      <c r="A48" s="77"/>
+      <c r="A48" s="78"/>
       <c r="B48" s="35" t="s">
         <v>120</v>
       </c>
@@ -12145,7 +12161,7 @@
       <c r="M48" s="51"/>
     </row>
     <row r="49" spans="1:13" ht="14.55" customHeight="1">
-      <c r="A49" s="77"/>
+      <c r="A49" s="78"/>
       <c r="B49" s="47" t="s">
         <v>194</v>
       </c>
@@ -12175,7 +12191,7 @@
       <c r="M49" s="51"/>
     </row>
     <row r="50" spans="1:13">
-      <c r="A50" s="77"/>
+      <c r="A50" s="78"/>
       <c r="B50" s="35" t="s">
         <v>21</v>
       </c>
@@ -12204,7 +12220,7 @@
       <c r="M50" s="51"/>
     </row>
     <row r="51" spans="1:13">
-      <c r="A51" s="77"/>
+      <c r="A51" s="78"/>
       <c r="B51" s="35" t="s">
         <v>22</v>
       </c>
@@ -12233,7 +12249,7 @@
       <c r="M51" s="51"/>
     </row>
     <row r="52" spans="1:13">
-      <c r="A52" s="77"/>
+      <c r="A52" s="78"/>
       <c r="B52" s="35" t="s">
         <v>23</v>
       </c>
@@ -12262,7 +12278,7 @@
       <c r="M52" s="51"/>
     </row>
     <row r="53" spans="1:13">
-      <c r="A53" s="78"/>
+      <c r="A53" s="79"/>
       <c r="B53" s="35" t="s">
         <v>138</v>
       </c>
@@ -12434,7 +12450,7 @@
       </c>
     </row>
     <row r="60" spans="1:13" ht="14.55" customHeight="1">
-      <c r="A60" s="79" t="s">
+      <c r="A60" s="62" t="s">
         <v>215</v>
       </c>
       <c r="B60" s="17" t="s">
@@ -12461,7 +12477,7 @@
       <c r="K60" s="13"/>
     </row>
     <row r="61" spans="1:13">
-      <c r="A61" s="62"/>
+      <c r="A61" s="63"/>
       <c r="B61" s="17" t="s">
         <v>218</v>
       </c>
@@ -12486,7 +12502,7 @@
       <c r="K61" s="13"/>
     </row>
     <row r="62" spans="1:13">
-      <c r="A62" s="62"/>
+      <c r="A62" s="63"/>
       <c r="B62" s="17" t="s">
         <v>219</v>
       </c>
@@ -12511,7 +12527,7 @@
       <c r="K62" s="13"/>
     </row>
     <row r="63" spans="1:13">
-      <c r="A63" s="62"/>
+      <c r="A63" s="63"/>
       <c r="B63" s="17" t="s">
         <v>220</v>
       </c>
@@ -12532,7 +12548,7 @@
       <c r="K63" s="13"/>
     </row>
     <row r="64" spans="1:13">
-      <c r="A64" s="62"/>
+      <c r="A64" s="63"/>
       <c r="B64" s="17" t="s">
         <v>221</v>
       </c>
@@ -12553,7 +12569,7 @@
       <c r="K64" s="13"/>
     </row>
     <row r="65" spans="1:11">
-      <c r="A65" s="62"/>
+      <c r="A65" s="63"/>
       <c r="B65" s="17" t="s">
         <v>222</v>
       </c>
@@ -12578,7 +12594,7 @@
       <c r="K65" s="13"/>
     </row>
     <row r="66" spans="1:11">
-      <c r="A66" s="62"/>
+      <c r="A66" s="63"/>
       <c r="B66" s="17" t="s">
         <v>223</v>
       </c>
@@ -12603,7 +12619,7 @@
       <c r="K66" s="13"/>
     </row>
     <row r="67" spans="1:11">
-      <c r="A67" s="62"/>
+      <c r="A67" s="63"/>
       <c r="B67" s="20" t="s">
         <v>224</v>
       </c>
@@ -12627,7 +12643,7 @@
       </c>
     </row>
     <row r="68" spans="1:11">
-      <c r="A68" s="62"/>
+      <c r="A68" s="63"/>
       <c r="B68" s="20" t="s">
         <v>225</v>
       </c>
@@ -12647,7 +12663,7 @@
       <c r="G68" s="19"/>
     </row>
     <row r="69" spans="1:11">
-      <c r="A69" s="62"/>
+      <c r="A69" s="63"/>
       <c r="B69" s="20" t="s">
         <v>226</v>
       </c>
@@ -12667,7 +12683,7 @@
       <c r="G69" s="19"/>
     </row>
     <row r="70" spans="1:11" ht="14.55" customHeight="1">
-      <c r="A70" s="79" t="s">
+      <c r="A70" s="62" t="s">
         <v>216</v>
       </c>
       <c r="B70" s="17" t="s">
@@ -12694,7 +12710,7 @@
       <c r="K70" s="13"/>
     </row>
     <row r="71" spans="1:11">
-      <c r="A71" s="62"/>
+      <c r="A71" s="63"/>
       <c r="B71" s="17" t="s">
         <v>228</v>
       </c>
@@ -12719,7 +12735,7 @@
       <c r="K71" s="13"/>
     </row>
     <row r="72" spans="1:11">
-      <c r="A72" s="62"/>
+      <c r="A72" s="63"/>
       <c r="B72" s="17" t="s">
         <v>229</v>
       </c>
@@ -12732,7 +12748,7 @@
         <v>4.1411112511024325E-3</v>
       </c>
       <c r="E72" s="18">
-        <f t="shared" ref="E72:E86" si="3">C72*1.1</f>
+        <f t="shared" ref="E72:E80" si="3">C72*1.1</f>
         <v>5.0613581957918621E-3</v>
       </c>
       <c r="F72" s="19" t="s">
@@ -12744,7 +12760,7 @@
       <c r="K72" s="13"/>
     </row>
     <row r="73" spans="1:11">
-      <c r="A73" s="62"/>
+      <c r="A73" s="63"/>
       <c r="B73" s="17" t="s">
         <v>230</v>
       </c>
@@ -12765,7 +12781,7 @@
       <c r="K73" s="13"/>
     </row>
     <row r="74" spans="1:11">
-      <c r="A74" s="62"/>
+      <c r="A74" s="63"/>
       <c r="B74" s="17" t="s">
         <v>231</v>
       </c>
@@ -12786,7 +12802,7 @@
       <c r="K74" s="13"/>
     </row>
     <row r="75" spans="1:11">
-      <c r="A75" s="62"/>
+      <c r="A75" s="63"/>
       <c r="B75" s="17" t="s">
         <v>232</v>
       </c>
@@ -12811,7 +12827,7 @@
       <c r="K75" s="13"/>
     </row>
     <row r="76" spans="1:11">
-      <c r="A76" s="62"/>
+      <c r="A76" s="63"/>
       <c r="B76" s="17" t="s">
         <v>233</v>
       </c>
@@ -12836,7 +12852,7 @@
       <c r="K76" s="13"/>
     </row>
     <row r="77" spans="1:11">
-      <c r="A77" s="62"/>
+      <c r="A77" s="63"/>
       <c r="B77" s="20" t="s">
         <v>234</v>
       </c>
@@ -12860,7 +12876,7 @@
       </c>
     </row>
     <row r="78" spans="1:11">
-      <c r="A78" s="62"/>
+      <c r="A78" s="63"/>
       <c r="B78" s="20" t="s">
         <v>235</v>
       </c>
@@ -12880,7 +12896,7 @@
       <c r="G78" s="19"/>
     </row>
     <row r="79" spans="1:11">
-      <c r="A79" s="62"/>
+      <c r="A79" s="63"/>
       <c r="B79" s="20" t="s">
         <v>236</v>
       </c>
@@ -12900,7 +12916,7 @@
       <c r="G79" s="19"/>
     </row>
     <row r="80" spans="1:11">
-      <c r="A80" s="62"/>
+      <c r="A80" s="63"/>
       <c r="B80" s="20" t="s">
         <v>117</v>
       </c>
@@ -12924,7 +12940,7 @@
       <c r="K80" s="13"/>
     </row>
     <row r="81" spans="1:11" ht="14.55" customHeight="1">
-      <c r="A81" s="62"/>
+      <c r="A81" s="63"/>
       <c r="B81" s="20" t="s">
         <v>159</v>
       </c>
@@ -12945,7 +12961,7 @@
       <c r="K81" s="13"/>
     </row>
     <row r="82" spans="1:11" ht="14.55" customHeight="1">
-      <c r="A82" s="62"/>
+      <c r="A82" s="63"/>
       <c r="B82" s="20" t="s">
         <v>206</v>
       </c>
@@ -12969,7 +12985,7 @@
       <c r="K82" s="13"/>
     </row>
     <row r="83" spans="1:11" ht="14.55" customHeight="1">
-      <c r="A83" s="62"/>
+      <c r="A83" s="63"/>
       <c r="B83" s="17" t="s">
         <v>161</v>
       </c>
@@ -12993,7 +13009,7 @@
       <c r="K83" s="13"/>
     </row>
     <row r="84" spans="1:11">
-      <c r="A84" s="62"/>
+      <c r="A84" s="63"/>
       <c r="B84" s="17" t="s">
         <v>162</v>
       </c>
@@ -13017,7 +13033,7 @@
       <c r="K84" s="13"/>
     </row>
     <row r="85" spans="1:11">
-      <c r="A85" s="62"/>
+      <c r="A85" s="63"/>
       <c r="B85" s="17" t="s">
         <v>164</v>
       </c>
@@ -13041,7 +13057,7 @@
       <c r="K85" s="13"/>
     </row>
     <row r="86" spans="1:11">
-      <c r="A86" s="63"/>
+      <c r="A86" s="64"/>
       <c r="B86" s="17" t="s">
         <v>76</v>
       </c>
@@ -13065,7 +13081,7 @@
       <c r="K86" s="13"/>
     </row>
     <row r="87" spans="1:11" ht="14.55" customHeight="1">
-      <c r="A87" s="64" t="s">
+      <c r="A87" s="65" t="s">
         <v>38</v>
       </c>
       <c r="B87" s="40" t="s">
@@ -13088,7 +13104,7 @@
       </c>
     </row>
     <row r="88" spans="1:11">
-      <c r="A88" s="65"/>
+      <c r="A88" s="66"/>
       <c r="B88" s="40" t="s">
         <v>48</v>
       </c>
@@ -13109,7 +13125,7 @@
       </c>
     </row>
     <row r="89" spans="1:11">
-      <c r="A89" s="65"/>
+      <c r="A89" s="66"/>
       <c r="B89" s="40" t="s">
         <v>40</v>
       </c>
@@ -13130,7 +13146,7 @@
       </c>
     </row>
     <row r="90" spans="1:11">
-      <c r="A90" s="65"/>
+      <c r="A90" s="66"/>
       <c r="B90" s="40" t="s">
         <v>41</v>
       </c>
@@ -13151,7 +13167,7 @@
       </c>
     </row>
     <row r="91" spans="1:11">
-      <c r="A91" s="65"/>
+      <c r="A91" s="66"/>
       <c r="B91" s="40" t="s">
         <v>42</v>
       </c>
@@ -13172,7 +13188,7 @@
       </c>
     </row>
     <row r="92" spans="1:11">
-      <c r="A92" s="65"/>
+      <c r="A92" s="66"/>
       <c r="B92" s="40" t="s">
         <v>188</v>
       </c>
@@ -13194,7 +13210,7 @@
       <c r="K92" s="13"/>
     </row>
     <row r="93" spans="1:11">
-      <c r="A93" s="65"/>
+      <c r="A93" s="66"/>
       <c r="B93" s="40" t="s">
         <v>43</v>
       </c>
@@ -13216,7 +13232,7 @@
       <c r="K93" s="13"/>
     </row>
     <row r="94" spans="1:11">
-      <c r="A94" s="65"/>
+      <c r="A94" s="66"/>
       <c r="B94" s="40" t="s">
         <v>49</v>
       </c>
@@ -13238,7 +13254,7 @@
       <c r="K94" s="13"/>
     </row>
     <row r="95" spans="1:11">
-      <c r="A95" s="65"/>
+      <c r="A95" s="66"/>
       <c r="B95" s="40" t="s">
         <v>44</v>
       </c>
@@ -13260,7 +13276,7 @@
       <c r="K95" s="13"/>
     </row>
     <row r="96" spans="1:11">
-      <c r="A96" s="65"/>
+      <c r="A96" s="66"/>
       <c r="B96" s="40" t="s">
         <v>45</v>
       </c>
@@ -13282,7 +13298,7 @@
       <c r="K96" s="13"/>
     </row>
     <row r="97" spans="1:11">
-      <c r="A97" s="65"/>
+      <c r="A97" s="66"/>
       <c r="B97" s="40" t="s">
         <v>46</v>
       </c>
@@ -13303,7 +13319,7 @@
       </c>
     </row>
     <row r="98" spans="1:11">
-      <c r="A98" s="65"/>
+      <c r="A98" s="66"/>
       <c r="B98" s="40" t="s">
         <v>189</v>
       </c>
@@ -13324,7 +13340,7 @@
       </c>
     </row>
     <row r="99" spans="1:11">
-      <c r="A99" s="65"/>
+      <c r="A99" s="66"/>
       <c r="B99" s="40" t="s">
         <v>47</v>
       </c>
@@ -13345,7 +13361,7 @@
       </c>
     </row>
     <row r="100" spans="1:11">
-      <c r="A100" s="65"/>
+      <c r="A100" s="66"/>
       <c r="B100" s="40" t="s">
         <v>50</v>
       </c>
@@ -13366,7 +13382,7 @@
       </c>
     </row>
     <row r="101" spans="1:11">
-      <c r="A101" s="65"/>
+      <c r="A101" s="66"/>
       <c r="B101" s="40" t="s">
         <v>51</v>
       </c>
@@ -13387,7 +13403,7 @@
       </c>
     </row>
     <row r="102" spans="1:11">
-      <c r="A102" s="65"/>
+      <c r="A102" s="66"/>
       <c r="B102" s="40" t="s">
         <v>52</v>
       </c>
@@ -13408,7 +13424,7 @@
       </c>
     </row>
     <row r="103" spans="1:11">
-      <c r="A103" s="65"/>
+      <c r="A103" s="66"/>
       <c r="B103" s="40" t="s">
         <v>53</v>
       </c>
@@ -13430,7 +13446,7 @@
       <c r="K103" s="13"/>
     </row>
     <row r="104" spans="1:11">
-      <c r="A104" s="65"/>
+      <c r="A104" s="66"/>
       <c r="B104" s="40" t="s">
         <v>190</v>
       </c>

</xml_diff>